<commit_message>
Mise à jour des consommations
</commit_message>
<xml_diff>
--- a/rapport_compteur.xlsx
+++ b/rapport_compteur.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="219">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -46,88 +46,7 @@
     <t xml:space="preserve">Inconnu</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-08-14 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-08-15 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-08-16 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-08-17 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-08-18 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-08-19 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-08-20 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-08-21 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-08-22 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-08-23 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-08-24 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-08-25 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-08-26 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-08-27 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-08-28 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-08-29 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-08-30 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-08-31 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-09-01 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-09-02 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-09-03 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-09-04 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-09-05 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-09-06 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-09-07 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-09-08 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-09-09 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-09-10 00:00:00 +0200</t>
+    <t xml:space="preserve">2023-09-10 23:30:00 +0200</t>
   </si>
   <si>
     <t xml:space="preserve">2023-09-11 00:00:00 +0200</t>
@@ -673,7 +592,91 @@
     <t xml:space="preserve">2024-04-08 00:00:00 +0200</t>
   </si>
   <si>
-    <t xml:space="preserve">2024-04-08 19:40:55 +0200</t>
+    <t xml:space="preserve">2024-04-09 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-10 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-11 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-12 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-13 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-14 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-15 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-16 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-17 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-18 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-19 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-20 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-21 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-22 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-23 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-24 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-25 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-26 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-27 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-28 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-29 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-30 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-01 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-02 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-03 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-04 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-05 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-06 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-06 19:05:54 +0200</t>
   </si>
 </sst>
 </file>
@@ -774,10 +777,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H211"/>
+  <dimension ref="A1:H212"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A172" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H213" activeCellId="0" sqref="H213"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -821,10 +824,10 @@
         <v>8</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>2695.536</v>
+        <v>2767.909</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>144.047</v>
+        <v>145.165</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>41.965</v>
@@ -847,10 +850,10 @@
         <v>9</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>2695.536</v>
+        <v>2767.917</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>144.047</v>
+        <v>145.165</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>41.965</v>
@@ -873,10 +876,10 @@
         <v>10</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>2695.536</v>
+        <v>2770.446</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>144.047</v>
+        <v>151.112</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>41.965</v>
@@ -899,10 +902,10 @@
         <v>11</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>2696.432</v>
+        <v>2770.446</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>144.047</v>
+        <v>151.112</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>41.965</v>
@@ -925,10 +928,10 @@
         <v>12</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>2696.432</v>
+        <v>2770.446</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>144.047</v>
+        <v>151.112</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>41.965</v>
@@ -951,10 +954,10 @@
         <v>13</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>2703.447</v>
+        <v>2770.446</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>144.047</v>
+        <v>151.112</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>41.965</v>
@@ -977,10 +980,10 @@
         <v>14</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>2722.556</v>
+        <v>2770.752</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>144.051</v>
+        <v>151.112</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>41.965</v>
@@ -1003,10 +1006,10 @@
         <v>15</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>2723.47</v>
+        <v>2770.752</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>144.051</v>
+        <v>151.112</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>41.965</v>
@@ -1029,10 +1032,10 @@
         <v>16</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>2723.47</v>
+        <v>2770.752</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>144.051</v>
+        <v>151.112</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>41.965</v>
@@ -1055,10 +1058,10 @@
         <v>17</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>2723.47</v>
+        <v>2771.824</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>144.051</v>
+        <v>151.112</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>41.965</v>
@@ -1081,10 +1084,10 @@
         <v>18</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>2723.678</v>
+        <v>2771.824</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>144.051</v>
+        <v>151.112</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>41.965</v>
@@ -1107,10 +1110,10 @@
         <v>19</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>2723.678</v>
+        <v>2771.951</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>144.051</v>
+        <v>151.112</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>41.965</v>
@@ -1133,10 +1136,10 @@
         <v>20</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>2723.678</v>
+        <v>2789.241</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>144.051</v>
+        <v>151.112</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>41.965</v>
@@ -1159,10 +1162,10 @@
         <v>21</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>2723.678</v>
+        <v>2811.081</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>144.051</v>
+        <v>151.112</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>41.965</v>
@@ -1185,10 +1188,10 @@
         <v>22</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>2724.521</v>
+        <v>2815.751</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>144.051</v>
+        <v>151.112</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>41.965</v>
@@ -1211,10 +1214,10 @@
         <v>23</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>2724.521</v>
+        <v>2838.684</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>144.051</v>
+        <v>157.472</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>41.965</v>
@@ -1237,10 +1240,10 @@
         <v>24</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>2724.521</v>
+        <v>2840.266</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>144.051</v>
+        <v>157.472</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>41.965</v>
@@ -1263,10 +1266,10 @@
         <v>25</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>2724.521</v>
+        <v>2840.531</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>144.051</v>
+        <v>157.472</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>41.965</v>
@@ -1289,10 +1292,10 @@
         <v>26</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>2724.778</v>
+        <v>2840.531</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>144.051</v>
+        <v>157.472</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>41.965</v>
@@ -1315,10 +1318,10 @@
         <v>27</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>2724.778</v>
+        <v>2840.843</v>
       </c>
       <c r="C21" s="0" t="n">
-        <v>144.051</v>
+        <v>157.472</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>41.965</v>
@@ -1341,10 +1344,10 @@
         <v>28</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>2725.696</v>
+        <v>2840.843</v>
       </c>
       <c r="C22" s="0" t="n">
-        <v>144.051</v>
+        <v>157.472</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>41.965</v>
@@ -1367,10 +1370,10 @@
         <v>29</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>2741.751</v>
+        <v>2840.843</v>
       </c>
       <c r="C23" s="0" t="n">
-        <v>144.051</v>
+        <v>157.472</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>41.965</v>
@@ -1393,10 +1396,10 @@
         <v>30</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>2741.751</v>
+        <v>2840.843</v>
       </c>
       <c r="C24" s="0" t="n">
-        <v>144.051</v>
+        <v>157.472</v>
       </c>
       <c r="D24" s="0" t="n">
         <v>41.965</v>
@@ -1419,10 +1422,10 @@
         <v>31</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>2741.751</v>
+        <v>2841.947</v>
       </c>
       <c r="C25" s="0" t="n">
-        <v>144.051</v>
+        <v>157.472</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>41.965</v>
@@ -1445,10 +1448,10 @@
         <v>32</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>2741.751</v>
+        <v>2841.947</v>
       </c>
       <c r="C26" s="0" t="n">
-        <v>144.051</v>
+        <v>157.472</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>41.965</v>
@@ -1471,10 +1474,10 @@
         <v>33</v>
       </c>
       <c r="B27" s="0" t="n">
-        <v>2741.751</v>
+        <v>2841.947</v>
       </c>
       <c r="C27" s="0" t="n">
-        <v>144.051</v>
+        <v>157.472</v>
       </c>
       <c r="D27" s="0" t="n">
         <v>41.965</v>
@@ -1497,10 +1500,10 @@
         <v>34</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>2741.751</v>
+        <v>2841.947</v>
       </c>
       <c r="C28" s="0" t="n">
-        <v>144.051</v>
+        <v>157.472</v>
       </c>
       <c r="D28" s="0" t="n">
         <v>41.965</v>
@@ -1523,10 +1526,10 @@
         <v>35</v>
       </c>
       <c r="B29" s="0" t="n">
-        <v>2744.934</v>
+        <v>2842.039</v>
       </c>
       <c r="C29" s="0" t="n">
-        <v>144.051</v>
+        <v>157.472</v>
       </c>
       <c r="D29" s="0" t="n">
         <v>41.965</v>
@@ -1549,10 +1552,10 @@
         <v>36</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>2767.917</v>
+        <v>2842.772</v>
       </c>
       <c r="C30" s="0" t="n">
-        <v>145.165</v>
+        <v>157.472</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>41.965</v>
@@ -1575,10 +1578,10 @@
         <v>37</v>
       </c>
       <c r="B31" s="0" t="n">
-        <v>2770.446</v>
+        <v>2842.772</v>
       </c>
       <c r="C31" s="0" t="n">
-        <v>151.112</v>
+        <v>157.472</v>
       </c>
       <c r="D31" s="0" t="n">
         <v>41.965</v>
@@ -1601,10 +1604,10 @@
         <v>38</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>2770.446</v>
+        <v>2842.772</v>
       </c>
       <c r="C32" s="0" t="n">
-        <v>151.112</v>
+        <v>157.472</v>
       </c>
       <c r="D32" s="0" t="n">
         <v>41.965</v>
@@ -1627,10 +1630,10 @@
         <v>39</v>
       </c>
       <c r="B33" s="0" t="n">
-        <v>2770.446</v>
+        <v>2842.772</v>
       </c>
       <c r="C33" s="0" t="n">
-        <v>151.112</v>
+        <v>157.472</v>
       </c>
       <c r="D33" s="0" t="n">
         <v>41.965</v>
@@ -1653,10 +1656,10 @@
         <v>40</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>2770.446</v>
+        <v>2842.772</v>
       </c>
       <c r="C34" s="0" t="n">
-        <v>151.112</v>
+        <v>157.472</v>
       </c>
       <c r="D34" s="0" t="n">
         <v>41.965</v>
@@ -1679,10 +1682,10 @@
         <v>41</v>
       </c>
       <c r="B35" s="0" t="n">
-        <v>2770.752</v>
+        <v>2842.772</v>
       </c>
       <c r="C35" s="0" t="n">
-        <v>151.112</v>
+        <v>157.472</v>
       </c>
       <c r="D35" s="0" t="n">
         <v>41.965</v>
@@ -1705,10 +1708,10 @@
         <v>42</v>
       </c>
       <c r="B36" s="0" t="n">
-        <v>2770.752</v>
+        <v>2842.772</v>
       </c>
       <c r="C36" s="0" t="n">
-        <v>151.112</v>
+        <v>157.472</v>
       </c>
       <c r="D36" s="0" t="n">
         <v>41.965</v>
@@ -1731,10 +1734,10 @@
         <v>43</v>
       </c>
       <c r="B37" s="0" t="n">
-        <v>2770.752</v>
+        <v>2842.772</v>
       </c>
       <c r="C37" s="0" t="n">
-        <v>151.112</v>
+        <v>157.472</v>
       </c>
       <c r="D37" s="0" t="n">
         <v>41.965</v>
@@ -1757,10 +1760,10 @@
         <v>44</v>
       </c>
       <c r="B38" s="0" t="n">
-        <v>2771.824</v>
+        <v>2843.983</v>
       </c>
       <c r="C38" s="0" t="n">
-        <v>151.112</v>
+        <v>157.472</v>
       </c>
       <c r="D38" s="0" t="n">
         <v>41.965</v>
@@ -1783,10 +1786,10 @@
         <v>45</v>
       </c>
       <c r="B39" s="0" t="n">
-        <v>2771.824</v>
+        <v>2843.983</v>
       </c>
       <c r="C39" s="0" t="n">
-        <v>151.112</v>
+        <v>157.472</v>
       </c>
       <c r="D39" s="0" t="n">
         <v>41.965</v>
@@ -1809,10 +1812,10 @@
         <v>46</v>
       </c>
       <c r="B40" s="0" t="n">
-        <v>2771.951</v>
+        <v>2843.983</v>
       </c>
       <c r="C40" s="0" t="n">
-        <v>151.112</v>
+        <v>157.472</v>
       </c>
       <c r="D40" s="0" t="n">
         <v>41.965</v>
@@ -1835,10 +1838,10 @@
         <v>47</v>
       </c>
       <c r="B41" s="0" t="n">
-        <v>2789.241</v>
+        <v>2843.983</v>
       </c>
       <c r="C41" s="0" t="n">
-        <v>151.112</v>
+        <v>157.472</v>
       </c>
       <c r="D41" s="0" t="n">
         <v>41.965</v>
@@ -1861,10 +1864,10 @@
         <v>48</v>
       </c>
       <c r="B42" s="0" t="n">
-        <v>2811.081</v>
+        <v>2843.983</v>
       </c>
       <c r="C42" s="0" t="n">
-        <v>151.112</v>
+        <v>157.472</v>
       </c>
       <c r="D42" s="0" t="n">
         <v>41.965</v>
@@ -1887,10 +1890,10 @@
         <v>49</v>
       </c>
       <c r="B43" s="0" t="n">
-        <v>2815.751</v>
+        <v>2843.983</v>
       </c>
       <c r="C43" s="0" t="n">
-        <v>151.112</v>
+        <v>157.472</v>
       </c>
       <c r="D43" s="0" t="n">
         <v>41.965</v>
@@ -1913,7 +1916,7 @@
         <v>50</v>
       </c>
       <c r="B44" s="0" t="n">
-        <v>2838.684</v>
+        <v>2845.039</v>
       </c>
       <c r="C44" s="0" t="n">
         <v>157.472</v>
@@ -1939,7 +1942,7 @@
         <v>51</v>
       </c>
       <c r="B45" s="0" t="n">
-        <v>2840.266</v>
+        <v>2845.039</v>
       </c>
       <c r="C45" s="0" t="n">
         <v>157.472</v>
@@ -1965,7 +1968,7 @@
         <v>52</v>
       </c>
       <c r="B46" s="0" t="n">
-        <v>2840.531</v>
+        <v>2845.039</v>
       </c>
       <c r="C46" s="0" t="n">
         <v>157.472</v>
@@ -1991,7 +1994,7 @@
         <v>53</v>
       </c>
       <c r="B47" s="0" t="n">
-        <v>2840.531</v>
+        <v>2845.039</v>
       </c>
       <c r="C47" s="0" t="n">
         <v>157.472</v>
@@ -2017,7 +2020,7 @@
         <v>54</v>
       </c>
       <c r="B48" s="0" t="n">
-        <v>2840.843</v>
+        <v>2845.039</v>
       </c>
       <c r="C48" s="0" t="n">
         <v>157.472</v>
@@ -2043,7 +2046,7 @@
         <v>55</v>
       </c>
       <c r="B49" s="0" t="n">
-        <v>2840.843</v>
+        <v>2845.039</v>
       </c>
       <c r="C49" s="0" t="n">
         <v>157.472</v>
@@ -2069,7 +2072,7 @@
         <v>56</v>
       </c>
       <c r="B50" s="0" t="n">
-        <v>2840.843</v>
+        <v>2845.039</v>
       </c>
       <c r="C50" s="0" t="n">
         <v>157.472</v>
@@ -2095,7 +2098,7 @@
         <v>57</v>
       </c>
       <c r="B51" s="0" t="n">
-        <v>2840.843</v>
+        <v>2845.039</v>
       </c>
       <c r="C51" s="0" t="n">
         <v>157.472</v>
@@ -2121,10 +2124,10 @@
         <v>58</v>
       </c>
       <c r="B52" s="0" t="n">
-        <v>2841.947</v>
+        <v>2862.022</v>
       </c>
       <c r="C52" s="0" t="n">
-        <v>157.472</v>
+        <v>157.518</v>
       </c>
       <c r="D52" s="0" t="n">
         <v>41.965</v>
@@ -2147,10 +2150,10 @@
         <v>59</v>
       </c>
       <c r="B53" s="0" t="n">
-        <v>2841.947</v>
+        <v>2862.034</v>
       </c>
       <c r="C53" s="0" t="n">
-        <v>157.472</v>
+        <v>157.619</v>
       </c>
       <c r="D53" s="0" t="n">
         <v>41.965</v>
@@ -2173,10 +2176,10 @@
         <v>60</v>
       </c>
       <c r="B54" s="0" t="n">
-        <v>2841.947</v>
+        <v>2863.113</v>
       </c>
       <c r="C54" s="0" t="n">
-        <v>157.472</v>
+        <v>157.619</v>
       </c>
       <c r="D54" s="0" t="n">
         <v>41.965</v>
@@ -2199,10 +2202,10 @@
         <v>61</v>
       </c>
       <c r="B55" s="0" t="n">
-        <v>2841.947</v>
+        <v>2863.113</v>
       </c>
       <c r="C55" s="0" t="n">
-        <v>157.472</v>
+        <v>157.619</v>
       </c>
       <c r="D55" s="0" t="n">
         <v>41.965</v>
@@ -2225,10 +2228,10 @@
         <v>62</v>
       </c>
       <c r="B56" s="0" t="n">
-        <v>2842.039</v>
+        <v>2863.113</v>
       </c>
       <c r="C56" s="0" t="n">
-        <v>157.472</v>
+        <v>157.619</v>
       </c>
       <c r="D56" s="0" t="n">
         <v>41.965</v>
@@ -2251,10 +2254,10 @@
         <v>63</v>
       </c>
       <c r="B57" s="0" t="n">
-        <v>2842.772</v>
+        <v>2863.113</v>
       </c>
       <c r="C57" s="0" t="n">
-        <v>157.472</v>
+        <v>157.619</v>
       </c>
       <c r="D57" s="0" t="n">
         <v>41.965</v>
@@ -2277,10 +2280,10 @@
         <v>64</v>
       </c>
       <c r="B58" s="0" t="n">
-        <v>2842.772</v>
+        <v>2863.331</v>
       </c>
       <c r="C58" s="0" t="n">
-        <v>157.472</v>
+        <v>157.619</v>
       </c>
       <c r="D58" s="0" t="n">
         <v>41.965</v>
@@ -2303,10 +2306,10 @@
         <v>65</v>
       </c>
       <c r="B59" s="0" t="n">
-        <v>2842.772</v>
+        <v>2863.721</v>
       </c>
       <c r="C59" s="0" t="n">
-        <v>157.472</v>
+        <v>157.619</v>
       </c>
       <c r="D59" s="0" t="n">
         <v>41.965</v>
@@ -2329,10 +2332,10 @@
         <v>66</v>
       </c>
       <c r="B60" s="0" t="n">
-        <v>2842.772</v>
+        <v>2863.721</v>
       </c>
       <c r="C60" s="0" t="n">
-        <v>157.472</v>
+        <v>157.619</v>
       </c>
       <c r="D60" s="0" t="n">
         <v>41.965</v>
@@ -2355,10 +2358,10 @@
         <v>67</v>
       </c>
       <c r="B61" s="0" t="n">
-        <v>2842.772</v>
+        <v>2864.183</v>
       </c>
       <c r="C61" s="0" t="n">
-        <v>157.472</v>
+        <v>157.619</v>
       </c>
       <c r="D61" s="0" t="n">
         <v>41.965</v>
@@ -2381,10 +2384,10 @@
         <v>68</v>
       </c>
       <c r="B62" s="0" t="n">
-        <v>2842.772</v>
+        <v>2864.183</v>
       </c>
       <c r="C62" s="0" t="n">
-        <v>157.472</v>
+        <v>157.619</v>
       </c>
       <c r="D62" s="0" t="n">
         <v>41.965</v>
@@ -2407,10 +2410,10 @@
         <v>69</v>
       </c>
       <c r="B63" s="0" t="n">
-        <v>2842.772</v>
+        <v>2864.404</v>
       </c>
       <c r="C63" s="0" t="n">
-        <v>157.472</v>
+        <v>157.619</v>
       </c>
       <c r="D63" s="0" t="n">
         <v>41.965</v>
@@ -2433,10 +2436,10 @@
         <v>70</v>
       </c>
       <c r="B64" s="0" t="n">
-        <v>2842.772</v>
+        <v>2864.404</v>
       </c>
       <c r="C64" s="0" t="n">
-        <v>157.472</v>
+        <v>157.619</v>
       </c>
       <c r="D64" s="0" t="n">
         <v>41.965</v>
@@ -2459,10 +2462,10 @@
         <v>71</v>
       </c>
       <c r="B65" s="0" t="n">
-        <v>2843.983</v>
+        <v>2875.844</v>
       </c>
       <c r="C65" s="0" t="n">
-        <v>157.472</v>
+        <v>157.619</v>
       </c>
       <c r="D65" s="0" t="n">
         <v>41.965</v>
@@ -2485,10 +2488,10 @@
         <v>72</v>
       </c>
       <c r="B66" s="0" t="n">
-        <v>2843.983</v>
+        <v>2875.844</v>
       </c>
       <c r="C66" s="0" t="n">
-        <v>157.472</v>
+        <v>157.619</v>
       </c>
       <c r="D66" s="0" t="n">
         <v>41.965</v>
@@ -2511,10 +2514,10 @@
         <v>73</v>
       </c>
       <c r="B67" s="0" t="n">
-        <v>2843.983</v>
+        <v>2875.844</v>
       </c>
       <c r="C67" s="0" t="n">
-        <v>157.472</v>
+        <v>157.619</v>
       </c>
       <c r="D67" s="0" t="n">
         <v>41.965</v>
@@ -2537,10 +2540,10 @@
         <v>74</v>
       </c>
       <c r="B68" s="0" t="n">
-        <v>2843.983</v>
+        <v>2875.844</v>
       </c>
       <c r="C68" s="0" t="n">
-        <v>157.472</v>
+        <v>157.619</v>
       </c>
       <c r="D68" s="0" t="n">
         <v>41.965</v>
@@ -2563,10 +2566,10 @@
         <v>75</v>
       </c>
       <c r="B69" s="0" t="n">
-        <v>2843.983</v>
+        <v>2875.853</v>
       </c>
       <c r="C69" s="0" t="n">
-        <v>157.472</v>
+        <v>157.619</v>
       </c>
       <c r="D69" s="0" t="n">
         <v>41.965</v>
@@ -2589,10 +2592,10 @@
         <v>76</v>
       </c>
       <c r="B70" s="0" t="n">
-        <v>2843.983</v>
+        <v>2876.161</v>
       </c>
       <c r="C70" s="0" t="n">
-        <v>157.472</v>
+        <v>157.619</v>
       </c>
       <c r="D70" s="0" t="n">
         <v>41.965</v>
@@ -2615,10 +2618,10 @@
         <v>77</v>
       </c>
       <c r="B71" s="0" t="n">
-        <v>2845.039</v>
+        <v>2876.161</v>
       </c>
       <c r="C71" s="0" t="n">
-        <v>157.472</v>
+        <v>157.619</v>
       </c>
       <c r="D71" s="0" t="n">
         <v>41.965</v>
@@ -2641,10 +2644,10 @@
         <v>78</v>
       </c>
       <c r="B72" s="0" t="n">
-        <v>2845.039</v>
+        <v>2876.397</v>
       </c>
       <c r="C72" s="0" t="n">
-        <v>157.472</v>
+        <v>157.619</v>
       </c>
       <c r="D72" s="0" t="n">
         <v>41.965</v>
@@ -2667,10 +2670,10 @@
         <v>79</v>
       </c>
       <c r="B73" s="0" t="n">
-        <v>2845.039</v>
+        <v>2886.936</v>
       </c>
       <c r="C73" s="0" t="n">
-        <v>157.472</v>
+        <v>157.782</v>
       </c>
       <c r="D73" s="0" t="n">
         <v>41.965</v>
@@ -2693,10 +2696,10 @@
         <v>80</v>
       </c>
       <c r="B74" s="0" t="n">
-        <v>2845.039</v>
+        <v>2887.492</v>
       </c>
       <c r="C74" s="0" t="n">
-        <v>157.472</v>
+        <v>157.782</v>
       </c>
       <c r="D74" s="0" t="n">
         <v>41.965</v>
@@ -2719,10 +2722,10 @@
         <v>81</v>
       </c>
       <c r="B75" s="0" t="n">
-        <v>2845.039</v>
+        <v>2887.771</v>
       </c>
       <c r="C75" s="0" t="n">
-        <v>157.472</v>
+        <v>157.782</v>
       </c>
       <c r="D75" s="0" t="n">
         <v>41.965</v>
@@ -2745,10 +2748,10 @@
         <v>82</v>
       </c>
       <c r="B76" s="0" t="n">
-        <v>2845.039</v>
+        <v>2887.771</v>
       </c>
       <c r="C76" s="0" t="n">
-        <v>157.472</v>
+        <v>157.782</v>
       </c>
       <c r="D76" s="0" t="n">
         <v>41.965</v>
@@ -2771,10 +2774,10 @@
         <v>83</v>
       </c>
       <c r="B77" s="0" t="n">
-        <v>2845.039</v>
+        <v>2887.771</v>
       </c>
       <c r="C77" s="0" t="n">
-        <v>157.472</v>
+        <v>157.782</v>
       </c>
       <c r="D77" s="0" t="n">
         <v>41.965</v>
@@ -2797,10 +2800,10 @@
         <v>84</v>
       </c>
       <c r="B78" s="0" t="n">
-        <v>2845.039</v>
+        <v>2888</v>
       </c>
       <c r="C78" s="0" t="n">
-        <v>157.472</v>
+        <v>157.782</v>
       </c>
       <c r="D78" s="0" t="n">
         <v>41.965</v>
@@ -2823,10 +2826,10 @@
         <v>85</v>
       </c>
       <c r="B79" s="0" t="n">
-        <v>2862.022</v>
+        <v>2888</v>
       </c>
       <c r="C79" s="0" t="n">
-        <v>157.518</v>
+        <v>157.782</v>
       </c>
       <c r="D79" s="0" t="n">
         <v>41.965</v>
@@ -2849,10 +2852,10 @@
         <v>86</v>
       </c>
       <c r="B80" s="0" t="n">
-        <v>2862.034</v>
+        <v>2899.866</v>
       </c>
       <c r="C80" s="0" t="n">
-        <v>157.619</v>
+        <v>157.782</v>
       </c>
       <c r="D80" s="0" t="n">
         <v>41.965</v>
@@ -2875,10 +2878,10 @@
         <v>87</v>
       </c>
       <c r="B81" s="0" t="n">
-        <v>2863.113</v>
+        <v>2899.866</v>
       </c>
       <c r="C81" s="0" t="n">
-        <v>157.619</v>
+        <v>157.782</v>
       </c>
       <c r="D81" s="0" t="n">
         <v>41.965</v>
@@ -2901,10 +2904,10 @@
         <v>88</v>
       </c>
       <c r="B82" s="0" t="n">
-        <v>2863.113</v>
+        <v>2899.866</v>
       </c>
       <c r="C82" s="0" t="n">
-        <v>157.619</v>
+        <v>157.782</v>
       </c>
       <c r="D82" s="0" t="n">
         <v>41.965</v>
@@ -2927,10 +2930,10 @@
         <v>89</v>
       </c>
       <c r="B83" s="0" t="n">
-        <v>2863.113</v>
+        <v>2899.866</v>
       </c>
       <c r="C83" s="0" t="n">
-        <v>157.619</v>
+        <v>157.782</v>
       </c>
       <c r="D83" s="0" t="n">
         <v>41.965</v>
@@ -2953,10 +2956,10 @@
         <v>90</v>
       </c>
       <c r="B84" s="0" t="n">
-        <v>2863.113</v>
+        <v>2899.866</v>
       </c>
       <c r="C84" s="0" t="n">
-        <v>157.619</v>
+        <v>157.782</v>
       </c>
       <c r="D84" s="0" t="n">
         <v>41.965</v>
@@ -2965,7 +2968,7 @@
         <v>2.256</v>
       </c>
       <c r="F84" s="0" t="n">
-        <v>2.942</v>
+        <v>3.311</v>
       </c>
       <c r="G84" s="0" t="n">
         <v>1.188</v>
@@ -2979,10 +2982,10 @@
         <v>91</v>
       </c>
       <c r="B85" s="0" t="n">
-        <v>2863.331</v>
+        <v>2899.866</v>
       </c>
       <c r="C85" s="0" t="n">
-        <v>157.619</v>
+        <v>157.782</v>
       </c>
       <c r="D85" s="0" t="n">
         <v>41.965</v>
@@ -2991,7 +2994,7 @@
         <v>2.256</v>
       </c>
       <c r="F85" s="0" t="n">
-        <v>2.942</v>
+        <v>3.311</v>
       </c>
       <c r="G85" s="0" t="n">
         <v>1.188</v>
@@ -3005,10 +3008,10 @@
         <v>92</v>
       </c>
       <c r="B86" s="0" t="n">
-        <v>2863.721</v>
+        <v>2899.866</v>
       </c>
       <c r="C86" s="0" t="n">
-        <v>157.619</v>
+        <v>157.782</v>
       </c>
       <c r="D86" s="0" t="n">
         <v>41.965</v>
@@ -3017,7 +3020,7 @@
         <v>2.256</v>
       </c>
       <c r="F86" s="0" t="n">
-        <v>2.942</v>
+        <v>3.563</v>
       </c>
       <c r="G86" s="0" t="n">
         <v>1.188</v>
@@ -3031,19 +3034,19 @@
         <v>93</v>
       </c>
       <c r="B87" s="0" t="n">
-        <v>2863.721</v>
+        <v>2899.866</v>
       </c>
       <c r="C87" s="0" t="n">
-        <v>157.619</v>
+        <v>157.782</v>
       </c>
       <c r="D87" s="0" t="n">
-        <v>41.965</v>
+        <v>42.191</v>
       </c>
       <c r="E87" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F87" s="0" t="n">
-        <v>2.942</v>
+        <v>3.563</v>
       </c>
       <c r="G87" s="0" t="n">
         <v>1.188</v>
@@ -3057,19 +3060,19 @@
         <v>94</v>
       </c>
       <c r="B88" s="0" t="n">
-        <v>2864.183</v>
+        <v>2899.866</v>
       </c>
       <c r="C88" s="0" t="n">
-        <v>157.619</v>
+        <v>157.782</v>
       </c>
       <c r="D88" s="0" t="n">
-        <v>41.965</v>
+        <v>42.191</v>
       </c>
       <c r="E88" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F88" s="0" t="n">
-        <v>2.942</v>
+        <v>3.563</v>
       </c>
       <c r="G88" s="0" t="n">
         <v>1.188</v>
@@ -3083,19 +3086,19 @@
         <v>95</v>
       </c>
       <c r="B89" s="0" t="n">
-        <v>2864.183</v>
+        <v>2900.388</v>
       </c>
       <c r="C89" s="0" t="n">
-        <v>157.619</v>
+        <v>157.782</v>
       </c>
       <c r="D89" s="0" t="n">
-        <v>41.965</v>
+        <v>42.191</v>
       </c>
       <c r="E89" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F89" s="0" t="n">
-        <v>2.942</v>
+        <v>3.563</v>
       </c>
       <c r="G89" s="0" t="n">
         <v>1.188</v>
@@ -3109,19 +3112,19 @@
         <v>96</v>
       </c>
       <c r="B90" s="0" t="n">
-        <v>2864.404</v>
+        <v>2900.388</v>
       </c>
       <c r="C90" s="0" t="n">
-        <v>157.619</v>
+        <v>157.782</v>
       </c>
       <c r="D90" s="0" t="n">
-        <v>41.965</v>
+        <v>42.191</v>
       </c>
       <c r="E90" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F90" s="0" t="n">
-        <v>2.942</v>
+        <v>3.563</v>
       </c>
       <c r="G90" s="0" t="n">
         <v>1.188</v>
@@ -3135,19 +3138,19 @@
         <v>97</v>
       </c>
       <c r="B91" s="0" t="n">
-        <v>2864.404</v>
+        <v>2900.388</v>
       </c>
       <c r="C91" s="0" t="n">
-        <v>157.619</v>
+        <v>157.782</v>
       </c>
       <c r="D91" s="0" t="n">
-        <v>41.965</v>
+        <v>42.191</v>
       </c>
       <c r="E91" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F91" s="0" t="n">
-        <v>2.942</v>
+        <v>3.793</v>
       </c>
       <c r="G91" s="0" t="n">
         <v>1.188</v>
@@ -3161,19 +3164,19 @@
         <v>98</v>
       </c>
       <c r="B92" s="0" t="n">
-        <v>2875.844</v>
+        <v>2900.388</v>
       </c>
       <c r="C92" s="0" t="n">
-        <v>157.619</v>
+        <v>157.782</v>
       </c>
       <c r="D92" s="0" t="n">
-        <v>41.965</v>
+        <v>42.416</v>
       </c>
       <c r="E92" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F92" s="0" t="n">
-        <v>2.942</v>
+        <v>3.793</v>
       </c>
       <c r="G92" s="0" t="n">
         <v>1.188</v>
@@ -3187,19 +3190,19 @@
         <v>99</v>
       </c>
       <c r="B93" s="0" t="n">
-        <v>2875.844</v>
+        <v>2900.388</v>
       </c>
       <c r="C93" s="0" t="n">
-        <v>157.619</v>
+        <v>157.835</v>
       </c>
       <c r="D93" s="0" t="n">
-        <v>41.965</v>
+        <v>42.65</v>
       </c>
       <c r="E93" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F93" s="0" t="n">
-        <v>2.942</v>
+        <v>3.793</v>
       </c>
       <c r="G93" s="0" t="n">
         <v>1.188</v>
@@ -3213,19 +3216,19 @@
         <v>100</v>
       </c>
       <c r="B94" s="0" t="n">
-        <v>2875.844</v>
+        <v>2912.717</v>
       </c>
       <c r="C94" s="0" t="n">
-        <v>157.619</v>
+        <v>159.561</v>
       </c>
       <c r="D94" s="0" t="n">
-        <v>41.965</v>
+        <v>42.65</v>
       </c>
       <c r="E94" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F94" s="0" t="n">
-        <v>2.942</v>
+        <v>3.793</v>
       </c>
       <c r="G94" s="0" t="n">
         <v>1.188</v>
@@ -3239,19 +3242,19 @@
         <v>101</v>
       </c>
       <c r="B95" s="0" t="n">
-        <v>2875.844</v>
+        <v>2924.242</v>
       </c>
       <c r="C95" s="0" t="n">
-        <v>157.619</v>
+        <v>159.561</v>
       </c>
       <c r="D95" s="0" t="n">
-        <v>41.965</v>
+        <v>42.65</v>
       </c>
       <c r="E95" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F95" s="0" t="n">
-        <v>2.942</v>
+        <v>3.793</v>
       </c>
       <c r="G95" s="0" t="n">
         <v>1.188</v>
@@ -3265,19 +3268,19 @@
         <v>102</v>
       </c>
       <c r="B96" s="0" t="n">
-        <v>2875.853</v>
+        <v>2924.242</v>
       </c>
       <c r="C96" s="0" t="n">
-        <v>157.619</v>
+        <v>159.561</v>
       </c>
       <c r="D96" s="0" t="n">
-        <v>41.965</v>
+        <v>42.65</v>
       </c>
       <c r="E96" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F96" s="0" t="n">
-        <v>2.942</v>
+        <v>3.793</v>
       </c>
       <c r="G96" s="0" t="n">
         <v>1.188</v>
@@ -3291,19 +3294,19 @@
         <v>103</v>
       </c>
       <c r="B97" s="0" t="n">
-        <v>2876.161</v>
+        <v>2924.242</v>
       </c>
       <c r="C97" s="0" t="n">
-        <v>157.619</v>
+        <v>159.561</v>
       </c>
       <c r="D97" s="0" t="n">
-        <v>41.965</v>
+        <v>42.65</v>
       </c>
       <c r="E97" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F97" s="0" t="n">
-        <v>2.942</v>
+        <v>3.793</v>
       </c>
       <c r="G97" s="0" t="n">
         <v>1.188</v>
@@ -3317,19 +3320,19 @@
         <v>104</v>
       </c>
       <c r="B98" s="0" t="n">
-        <v>2876.161</v>
+        <v>2924.242</v>
       </c>
       <c r="C98" s="0" t="n">
-        <v>157.619</v>
+        <v>159.561</v>
       </c>
       <c r="D98" s="0" t="n">
-        <v>41.965</v>
+        <v>42.65</v>
       </c>
       <c r="E98" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F98" s="0" t="n">
-        <v>2.942</v>
+        <v>3.793</v>
       </c>
       <c r="G98" s="0" t="n">
         <v>1.188</v>
@@ -3343,19 +3346,19 @@
         <v>105</v>
       </c>
       <c r="B99" s="0" t="n">
-        <v>2876.397</v>
+        <v>2924.242</v>
       </c>
       <c r="C99" s="0" t="n">
-        <v>157.619</v>
+        <v>159.561</v>
       </c>
       <c r="D99" s="0" t="n">
-        <v>41.965</v>
+        <v>42.665</v>
       </c>
       <c r="E99" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F99" s="0" t="n">
-        <v>2.942</v>
+        <v>3.793</v>
       </c>
       <c r="G99" s="0" t="n">
         <v>1.188</v>
@@ -3369,19 +3372,19 @@
         <v>106</v>
       </c>
       <c r="B100" s="0" t="n">
-        <v>2886.936</v>
+        <v>2924.242</v>
       </c>
       <c r="C100" s="0" t="n">
-        <v>157.782</v>
+        <v>159.561</v>
       </c>
       <c r="D100" s="0" t="n">
-        <v>41.965</v>
+        <v>42.665</v>
       </c>
       <c r="E100" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F100" s="0" t="n">
-        <v>2.942</v>
+        <v>3.793</v>
       </c>
       <c r="G100" s="0" t="n">
         <v>1.188</v>
@@ -3395,19 +3398,19 @@
         <v>107</v>
       </c>
       <c r="B101" s="0" t="n">
-        <v>2887.492</v>
+        <v>2931.72</v>
       </c>
       <c r="C101" s="0" t="n">
-        <v>157.782</v>
+        <v>159.561</v>
       </c>
       <c r="D101" s="0" t="n">
-        <v>41.965</v>
+        <v>43.124</v>
       </c>
       <c r="E101" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F101" s="0" t="n">
-        <v>2.942</v>
+        <v>3.793</v>
       </c>
       <c r="G101" s="0" t="n">
         <v>1.188</v>
@@ -3421,19 +3424,19 @@
         <v>108</v>
       </c>
       <c r="B102" s="0" t="n">
-        <v>2887.771</v>
+        <v>2950.048</v>
       </c>
       <c r="C102" s="0" t="n">
-        <v>157.782</v>
+        <v>159.561</v>
       </c>
       <c r="D102" s="0" t="n">
-        <v>41.965</v>
+        <v>43.124</v>
       </c>
       <c r="E102" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F102" s="0" t="n">
-        <v>2.942</v>
+        <v>3.793</v>
       </c>
       <c r="G102" s="0" t="n">
         <v>1.188</v>
@@ -3447,19 +3450,19 @@
         <v>109</v>
       </c>
       <c r="B103" s="0" t="n">
-        <v>2887.771</v>
+        <v>2950.048</v>
       </c>
       <c r="C103" s="0" t="n">
-        <v>157.782</v>
+        <v>159.561</v>
       </c>
       <c r="D103" s="0" t="n">
-        <v>41.965</v>
+        <v>43.729</v>
       </c>
       <c r="E103" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F103" s="0" t="n">
-        <v>2.942</v>
+        <v>3.793</v>
       </c>
       <c r="G103" s="0" t="n">
         <v>1.188</v>
@@ -3473,19 +3476,19 @@
         <v>110</v>
       </c>
       <c r="B104" s="0" t="n">
-        <v>2887.771</v>
+        <v>2950.048</v>
       </c>
       <c r="C104" s="0" t="n">
-        <v>157.782</v>
+        <v>159.561</v>
       </c>
       <c r="D104" s="0" t="n">
-        <v>41.965</v>
+        <v>43.729</v>
       </c>
       <c r="E104" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F104" s="0" t="n">
-        <v>2.942</v>
+        <v>3.793</v>
       </c>
       <c r="G104" s="0" t="n">
         <v>1.188</v>
@@ -3499,19 +3502,19 @@
         <v>111</v>
       </c>
       <c r="B105" s="0" t="n">
-        <v>2888</v>
+        <v>2950.356</v>
       </c>
       <c r="C105" s="0" t="n">
-        <v>157.782</v>
+        <v>159.561</v>
       </c>
       <c r="D105" s="0" t="n">
-        <v>41.965</v>
+        <v>43.729</v>
       </c>
       <c r="E105" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F105" s="0" t="n">
-        <v>2.942</v>
+        <v>3.793</v>
       </c>
       <c r="G105" s="0" t="n">
         <v>1.188</v>
@@ -3525,19 +3528,19 @@
         <v>112</v>
       </c>
       <c r="B106" s="0" t="n">
-        <v>2888</v>
+        <v>2950.356</v>
       </c>
       <c r="C106" s="0" t="n">
-        <v>157.782</v>
+        <v>159.561</v>
       </c>
       <c r="D106" s="0" t="n">
-        <v>41.965</v>
+        <v>43.729</v>
       </c>
       <c r="E106" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F106" s="0" t="n">
-        <v>2.942</v>
+        <v>3.793</v>
       </c>
       <c r="G106" s="0" t="n">
         <v>1.188</v>
@@ -3551,19 +3554,19 @@
         <v>113</v>
       </c>
       <c r="B107" s="0" t="n">
-        <v>2899.866</v>
+        <v>2963.804</v>
       </c>
       <c r="C107" s="0" t="n">
-        <v>157.782</v>
+        <v>164.049</v>
       </c>
       <c r="D107" s="0" t="n">
-        <v>41.965</v>
+        <v>43.729</v>
       </c>
       <c r="E107" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F107" s="0" t="n">
-        <v>2.942</v>
+        <v>3.793</v>
       </c>
       <c r="G107" s="0" t="n">
         <v>1.188</v>
@@ -3577,19 +3580,19 @@
         <v>114</v>
       </c>
       <c r="B108" s="0" t="n">
-        <v>2899.866</v>
+        <v>2963.804</v>
       </c>
       <c r="C108" s="0" t="n">
-        <v>157.782</v>
+        <v>164.049</v>
       </c>
       <c r="D108" s="0" t="n">
-        <v>41.965</v>
+        <v>43.729</v>
       </c>
       <c r="E108" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F108" s="0" t="n">
-        <v>2.942</v>
+        <v>3.793</v>
       </c>
       <c r="G108" s="0" t="n">
         <v>1.188</v>
@@ -3603,19 +3606,19 @@
         <v>115</v>
       </c>
       <c r="B109" s="0" t="n">
-        <v>2899.866</v>
+        <v>2963.804</v>
       </c>
       <c r="C109" s="0" t="n">
-        <v>157.782</v>
+        <v>164.049</v>
       </c>
       <c r="D109" s="0" t="n">
-        <v>41.965</v>
+        <v>43.729</v>
       </c>
       <c r="E109" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F109" s="0" t="n">
-        <v>2.942</v>
+        <v>3.793</v>
       </c>
       <c r="G109" s="0" t="n">
         <v>1.188</v>
@@ -3629,19 +3632,19 @@
         <v>116</v>
       </c>
       <c r="B110" s="0" t="n">
-        <v>2899.866</v>
+        <v>2971.367</v>
       </c>
       <c r="C110" s="0" t="n">
-        <v>157.782</v>
+        <v>164.049</v>
       </c>
       <c r="D110" s="0" t="n">
-        <v>41.965</v>
+        <v>43.729</v>
       </c>
       <c r="E110" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F110" s="0" t="n">
-        <v>2.942</v>
+        <v>3.793</v>
       </c>
       <c r="G110" s="0" t="n">
         <v>1.188</v>
@@ -3655,19 +3658,19 @@
         <v>117</v>
       </c>
       <c r="B111" s="0" t="n">
-        <v>2899.866</v>
+        <v>2980.453</v>
       </c>
       <c r="C111" s="0" t="n">
-        <v>157.782</v>
+        <v>164.049</v>
       </c>
       <c r="D111" s="0" t="n">
-        <v>41.965</v>
+        <v>43.729</v>
       </c>
       <c r="E111" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F111" s="0" t="n">
-        <v>3.311</v>
+        <v>3.793</v>
       </c>
       <c r="G111" s="0" t="n">
         <v>1.188</v>
@@ -3681,19 +3684,19 @@
         <v>118</v>
       </c>
       <c r="B112" s="0" t="n">
-        <v>2899.866</v>
+        <v>2997.787</v>
       </c>
       <c r="C112" s="0" t="n">
-        <v>157.782</v>
+        <v>164.049</v>
       </c>
       <c r="D112" s="0" t="n">
-        <v>41.965</v>
+        <v>43.729</v>
       </c>
       <c r="E112" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F112" s="0" t="n">
-        <v>3.311</v>
+        <v>3.793</v>
       </c>
       <c r="G112" s="0" t="n">
         <v>1.188</v>
@@ -3707,19 +3710,19 @@
         <v>119</v>
       </c>
       <c r="B113" s="0" t="n">
-        <v>2899.866</v>
+        <v>2997.787</v>
       </c>
       <c r="C113" s="0" t="n">
-        <v>157.782</v>
+        <v>164.049</v>
       </c>
       <c r="D113" s="0" t="n">
-        <v>41.965</v>
+        <v>43.729</v>
       </c>
       <c r="E113" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F113" s="0" t="n">
-        <v>3.563</v>
+        <v>3.793</v>
       </c>
       <c r="G113" s="0" t="n">
         <v>1.188</v>
@@ -3733,19 +3736,19 @@
         <v>120</v>
       </c>
       <c r="B114" s="0" t="n">
-        <v>2899.866</v>
+        <v>2997.787</v>
       </c>
       <c r="C114" s="0" t="n">
-        <v>157.782</v>
+        <v>164.049</v>
       </c>
       <c r="D114" s="0" t="n">
-        <v>42.191</v>
+        <v>43.729</v>
       </c>
       <c r="E114" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F114" s="0" t="n">
-        <v>3.563</v>
+        <v>3.793</v>
       </c>
       <c r="G114" s="0" t="n">
         <v>1.188</v>
@@ -3759,19 +3762,19 @@
         <v>121</v>
       </c>
       <c r="B115" s="0" t="n">
-        <v>2899.866</v>
+        <v>2997.787</v>
       </c>
       <c r="C115" s="0" t="n">
-        <v>157.782</v>
+        <v>164.049</v>
       </c>
       <c r="D115" s="0" t="n">
-        <v>42.191</v>
+        <v>43.729</v>
       </c>
       <c r="E115" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F115" s="0" t="n">
-        <v>3.563</v>
+        <v>3.793</v>
       </c>
       <c r="G115" s="0" t="n">
         <v>1.188</v>
@@ -3785,19 +3788,19 @@
         <v>122</v>
       </c>
       <c r="B116" s="0" t="n">
-        <v>2900.388</v>
+        <v>2997.787</v>
       </c>
       <c r="C116" s="0" t="n">
-        <v>157.782</v>
+        <v>164.049</v>
       </c>
       <c r="D116" s="0" t="n">
-        <v>42.191</v>
+        <v>43.729</v>
       </c>
       <c r="E116" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F116" s="0" t="n">
-        <v>3.563</v>
+        <v>3.793</v>
       </c>
       <c r="G116" s="0" t="n">
         <v>1.188</v>
@@ -3811,19 +3814,19 @@
         <v>123</v>
       </c>
       <c r="B117" s="0" t="n">
-        <v>2900.388</v>
+        <v>2997.787</v>
       </c>
       <c r="C117" s="0" t="n">
-        <v>157.782</v>
+        <v>164.049</v>
       </c>
       <c r="D117" s="0" t="n">
-        <v>42.191</v>
+        <v>43.729</v>
       </c>
       <c r="E117" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F117" s="0" t="n">
-        <v>3.563</v>
+        <v>3.793</v>
       </c>
       <c r="G117" s="0" t="n">
         <v>1.188</v>
@@ -3837,13 +3840,13 @@
         <v>124</v>
       </c>
       <c r="B118" s="0" t="n">
-        <v>2900.388</v>
+        <v>2997.787</v>
       </c>
       <c r="C118" s="0" t="n">
-        <v>157.782</v>
+        <v>164.049</v>
       </c>
       <c r="D118" s="0" t="n">
-        <v>42.191</v>
+        <v>43.729</v>
       </c>
       <c r="E118" s="0" t="n">
         <v>2.256</v>
@@ -3863,13 +3866,13 @@
         <v>125</v>
       </c>
       <c r="B119" s="0" t="n">
-        <v>2900.388</v>
+        <v>2997.787</v>
       </c>
       <c r="C119" s="0" t="n">
-        <v>157.782</v>
+        <v>164.049</v>
       </c>
       <c r="D119" s="0" t="n">
-        <v>42.416</v>
+        <v>43.729</v>
       </c>
       <c r="E119" s="0" t="n">
         <v>2.256</v>
@@ -3889,13 +3892,13 @@
         <v>126</v>
       </c>
       <c r="B120" s="0" t="n">
-        <v>2900.388</v>
+        <v>2997.787</v>
       </c>
       <c r="C120" s="0" t="n">
-        <v>157.835</v>
+        <v>164.049</v>
       </c>
       <c r="D120" s="0" t="n">
-        <v>42.65</v>
+        <v>43.729</v>
       </c>
       <c r="E120" s="0" t="n">
         <v>2.256</v>
@@ -3915,13 +3918,13 @@
         <v>127</v>
       </c>
       <c r="B121" s="0" t="n">
-        <v>2912.717</v>
+        <v>2997.787</v>
       </c>
       <c r="C121" s="0" t="n">
-        <v>159.561</v>
+        <v>164.049</v>
       </c>
       <c r="D121" s="0" t="n">
-        <v>42.65</v>
+        <v>43.736</v>
       </c>
       <c r="E121" s="0" t="n">
         <v>2.256</v>
@@ -3941,13 +3944,13 @@
         <v>128</v>
       </c>
       <c r="B122" s="0" t="n">
-        <v>2924.242</v>
+        <v>2997.937</v>
       </c>
       <c r="C122" s="0" t="n">
-        <v>159.561</v>
+        <v>164.049</v>
       </c>
       <c r="D122" s="0" t="n">
-        <v>42.65</v>
+        <v>43.736</v>
       </c>
       <c r="E122" s="0" t="n">
         <v>2.256</v>
@@ -3967,13 +3970,13 @@
         <v>129</v>
       </c>
       <c r="B123" s="0" t="n">
-        <v>2924.242</v>
+        <v>2997.937</v>
       </c>
       <c r="C123" s="0" t="n">
-        <v>159.561</v>
+        <v>164.049</v>
       </c>
       <c r="D123" s="0" t="n">
-        <v>42.65</v>
+        <v>43.736</v>
       </c>
       <c r="E123" s="0" t="n">
         <v>2.256</v>
@@ -3993,19 +3996,19 @@
         <v>130</v>
       </c>
       <c r="B124" s="0" t="n">
-        <v>2924.242</v>
+        <v>2997.937</v>
       </c>
       <c r="C124" s="0" t="n">
-        <v>159.561</v>
+        <v>164.049</v>
       </c>
       <c r="D124" s="0" t="n">
-        <v>42.65</v>
+        <v>43.736</v>
       </c>
       <c r="E124" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F124" s="0" t="n">
-        <v>3.793</v>
+        <v>4.549</v>
       </c>
       <c r="G124" s="0" t="n">
         <v>1.188</v>
@@ -4019,19 +4022,19 @@
         <v>131</v>
       </c>
       <c r="B125" s="0" t="n">
-        <v>2924.242</v>
+        <v>2997.937</v>
       </c>
       <c r="C125" s="0" t="n">
-        <v>159.561</v>
+        <v>164.049</v>
       </c>
       <c r="D125" s="0" t="n">
-        <v>42.65</v>
+        <v>43.736</v>
       </c>
       <c r="E125" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F125" s="0" t="n">
-        <v>3.793</v>
+        <v>4.949</v>
       </c>
       <c r="G125" s="0" t="n">
         <v>1.188</v>
@@ -4045,19 +4048,19 @@
         <v>132</v>
       </c>
       <c r="B126" s="0" t="n">
-        <v>2924.242</v>
+        <v>2997.937</v>
       </c>
       <c r="C126" s="0" t="n">
-        <v>159.561</v>
+        <v>164.049</v>
       </c>
       <c r="D126" s="0" t="n">
-        <v>42.665</v>
+        <v>43.736</v>
       </c>
       <c r="E126" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F126" s="0" t="n">
-        <v>3.793</v>
+        <v>4.949</v>
       </c>
       <c r="G126" s="0" t="n">
         <v>1.188</v>
@@ -4071,19 +4074,19 @@
         <v>133</v>
       </c>
       <c r="B127" s="0" t="n">
-        <v>2924.242</v>
+        <v>2997.937</v>
       </c>
       <c r="C127" s="0" t="n">
-        <v>159.561</v>
+        <v>164.049</v>
       </c>
       <c r="D127" s="0" t="n">
-        <v>42.665</v>
+        <v>43.736</v>
       </c>
       <c r="E127" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F127" s="0" t="n">
-        <v>3.793</v>
+        <v>4.949</v>
       </c>
       <c r="G127" s="0" t="n">
         <v>1.188</v>
@@ -4097,19 +4100,19 @@
         <v>134</v>
       </c>
       <c r="B128" s="0" t="n">
-        <v>2931.72</v>
+        <v>2997.937</v>
       </c>
       <c r="C128" s="0" t="n">
-        <v>159.561</v>
+        <v>164.049</v>
       </c>
       <c r="D128" s="0" t="n">
-        <v>43.124</v>
+        <v>43.736</v>
       </c>
       <c r="E128" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F128" s="0" t="n">
-        <v>3.793</v>
+        <v>4.949</v>
       </c>
       <c r="G128" s="0" t="n">
         <v>1.188</v>
@@ -4123,19 +4126,19 @@
         <v>135</v>
       </c>
       <c r="B129" s="0" t="n">
-        <v>2950.048</v>
+        <v>3005.43</v>
       </c>
       <c r="C129" s="0" t="n">
-        <v>159.561</v>
+        <v>164.049</v>
       </c>
       <c r="D129" s="0" t="n">
-        <v>43.124</v>
+        <v>43.736</v>
       </c>
       <c r="E129" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F129" s="0" t="n">
-        <v>3.793</v>
+        <v>4.949</v>
       </c>
       <c r="G129" s="0" t="n">
         <v>1.188</v>
@@ -4149,19 +4152,19 @@
         <v>136</v>
       </c>
       <c r="B130" s="0" t="n">
-        <v>2950.048</v>
+        <v>3010.782</v>
       </c>
       <c r="C130" s="0" t="n">
-        <v>159.561</v>
+        <v>164.049</v>
       </c>
       <c r="D130" s="0" t="n">
-        <v>43.729</v>
+        <v>43.736</v>
       </c>
       <c r="E130" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F130" s="0" t="n">
-        <v>3.793</v>
+        <v>4.949</v>
       </c>
       <c r="G130" s="0" t="n">
         <v>1.188</v>
@@ -4175,19 +4178,19 @@
         <v>137</v>
       </c>
       <c r="B131" s="0" t="n">
-        <v>2950.048</v>
+        <v>3010.782</v>
       </c>
       <c r="C131" s="0" t="n">
-        <v>159.561</v>
+        <v>164.049</v>
       </c>
       <c r="D131" s="0" t="n">
-        <v>43.729</v>
+        <v>43.736</v>
       </c>
       <c r="E131" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F131" s="0" t="n">
-        <v>3.793</v>
+        <v>4.949</v>
       </c>
       <c r="G131" s="0" t="n">
         <v>1.188</v>
@@ -4201,19 +4204,19 @@
         <v>138</v>
       </c>
       <c r="B132" s="0" t="n">
-        <v>2950.356</v>
+        <v>3010.782</v>
       </c>
       <c r="C132" s="0" t="n">
-        <v>159.561</v>
+        <v>164.049</v>
       </c>
       <c r="D132" s="0" t="n">
-        <v>43.729</v>
+        <v>43.971</v>
       </c>
       <c r="E132" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F132" s="0" t="n">
-        <v>3.793</v>
+        <v>4.949</v>
       </c>
       <c r="G132" s="0" t="n">
         <v>1.188</v>
@@ -4227,19 +4230,19 @@
         <v>139</v>
       </c>
       <c r="B133" s="0" t="n">
-        <v>2950.356</v>
+        <v>3010.782</v>
       </c>
       <c r="C133" s="0" t="n">
-        <v>159.561</v>
+        <v>164.049</v>
       </c>
       <c r="D133" s="0" t="n">
-        <v>43.729</v>
+        <v>43.971</v>
       </c>
       <c r="E133" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F133" s="0" t="n">
-        <v>3.793</v>
+        <v>5.216</v>
       </c>
       <c r="G133" s="0" t="n">
         <v>1.188</v>
@@ -4253,19 +4256,19 @@
         <v>140</v>
       </c>
       <c r="B134" s="0" t="n">
-        <v>2963.804</v>
+        <v>3010.782</v>
       </c>
       <c r="C134" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D134" s="0" t="n">
-        <v>43.729</v>
+        <v>43.971</v>
       </c>
       <c r="E134" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F134" s="0" t="n">
-        <v>3.793</v>
+        <v>5.442</v>
       </c>
       <c r="G134" s="0" t="n">
         <v>1.188</v>
@@ -4279,19 +4282,19 @@
         <v>141</v>
       </c>
       <c r="B135" s="0" t="n">
-        <v>2963.804</v>
+        <v>3010.782</v>
       </c>
       <c r="C135" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D135" s="0" t="n">
-        <v>43.729</v>
+        <v>43.971</v>
       </c>
       <c r="E135" s="0" t="n">
-        <v>2.256</v>
+        <v>2.362</v>
       </c>
       <c r="F135" s="0" t="n">
-        <v>3.793</v>
+        <v>5.442</v>
       </c>
       <c r="G135" s="0" t="n">
         <v>1.188</v>
@@ -4305,19 +4308,19 @@
         <v>142</v>
       </c>
       <c r="B136" s="0" t="n">
-        <v>2963.804</v>
+        <v>3018.213</v>
       </c>
       <c r="C136" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D136" s="0" t="n">
-        <v>43.729</v>
+        <v>43.971</v>
       </c>
       <c r="E136" s="0" t="n">
-        <v>2.256</v>
+        <v>2.362</v>
       </c>
       <c r="F136" s="0" t="n">
-        <v>3.793</v>
+        <v>5.442</v>
       </c>
       <c r="G136" s="0" t="n">
         <v>1.188</v>
@@ -4331,19 +4334,19 @@
         <v>143</v>
       </c>
       <c r="B137" s="0" t="n">
-        <v>2971.367</v>
+        <v>3027.483</v>
       </c>
       <c r="C137" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D137" s="0" t="n">
-        <v>43.729</v>
+        <v>43.971</v>
       </c>
       <c r="E137" s="0" t="n">
-        <v>2.256</v>
+        <v>2.362</v>
       </c>
       <c r="F137" s="0" t="n">
-        <v>3.793</v>
+        <v>5.442</v>
       </c>
       <c r="G137" s="0" t="n">
         <v>1.188</v>
@@ -4357,19 +4360,19 @@
         <v>144</v>
       </c>
       <c r="B138" s="0" t="n">
-        <v>2980.453</v>
+        <v>3037.77</v>
       </c>
       <c r="C138" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D138" s="0" t="n">
-        <v>43.729</v>
+        <v>43.971</v>
       </c>
       <c r="E138" s="0" t="n">
-        <v>2.256</v>
+        <v>2.362</v>
       </c>
       <c r="F138" s="0" t="n">
-        <v>3.793</v>
+        <v>5.442</v>
       </c>
       <c r="G138" s="0" t="n">
         <v>1.188</v>
@@ -4383,19 +4386,19 @@
         <v>145</v>
       </c>
       <c r="B139" s="0" t="n">
-        <v>2997.787</v>
+        <v>3037.77</v>
       </c>
       <c r="C139" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D139" s="0" t="n">
-        <v>43.729</v>
+        <v>43.971</v>
       </c>
       <c r="E139" s="0" t="n">
-        <v>2.256</v>
+        <v>2.362</v>
       </c>
       <c r="F139" s="0" t="n">
-        <v>3.793</v>
+        <v>5.442</v>
       </c>
       <c r="G139" s="0" t="n">
         <v>1.188</v>
@@ -4409,19 +4412,19 @@
         <v>146</v>
       </c>
       <c r="B140" s="0" t="n">
-        <v>2997.787</v>
+        <v>3037.77</v>
       </c>
       <c r="C140" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D140" s="0" t="n">
-        <v>43.729</v>
+        <v>43.971</v>
       </c>
       <c r="E140" s="0" t="n">
-        <v>2.256</v>
+        <v>2.362</v>
       </c>
       <c r="F140" s="0" t="n">
-        <v>3.793</v>
+        <v>5.442</v>
       </c>
       <c r="G140" s="0" t="n">
         <v>1.188</v>
@@ -4435,19 +4438,19 @@
         <v>147</v>
       </c>
       <c r="B141" s="0" t="n">
-        <v>2997.787</v>
+        <v>3037.77</v>
       </c>
       <c r="C141" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D141" s="0" t="n">
-        <v>43.729</v>
+        <v>43.979</v>
       </c>
       <c r="E141" s="0" t="n">
-        <v>2.256</v>
+        <v>2.362</v>
       </c>
       <c r="F141" s="0" t="n">
-        <v>3.793</v>
+        <v>5.442</v>
       </c>
       <c r="G141" s="0" t="n">
         <v>1.188</v>
@@ -4461,19 +4464,19 @@
         <v>148</v>
       </c>
       <c r="B142" s="0" t="n">
-        <v>2997.787</v>
+        <v>3045.333</v>
       </c>
       <c r="C142" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D142" s="0" t="n">
-        <v>43.729</v>
+        <v>43.979</v>
       </c>
       <c r="E142" s="0" t="n">
-        <v>2.256</v>
+        <v>2.362</v>
       </c>
       <c r="F142" s="0" t="n">
-        <v>3.793</v>
+        <v>5.442</v>
       </c>
       <c r="G142" s="0" t="n">
         <v>1.188</v>
@@ -4487,19 +4490,19 @@
         <v>149</v>
       </c>
       <c r="B143" s="0" t="n">
-        <v>2997.787</v>
+        <v>3067.38</v>
       </c>
       <c r="C143" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D143" s="0" t="n">
-        <v>43.729</v>
+        <v>43.979</v>
       </c>
       <c r="E143" s="0" t="n">
-        <v>2.256</v>
+        <v>2.362</v>
       </c>
       <c r="F143" s="0" t="n">
-        <v>3.793</v>
+        <v>5.442</v>
       </c>
       <c r="G143" s="0" t="n">
         <v>1.188</v>
@@ -4513,19 +4516,19 @@
         <v>150</v>
       </c>
       <c r="B144" s="0" t="n">
-        <v>2997.787</v>
+        <v>3067.38</v>
       </c>
       <c r="C144" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D144" s="0" t="n">
-        <v>43.729</v>
+        <v>44.017</v>
       </c>
       <c r="E144" s="0" t="n">
-        <v>2.256</v>
+        <v>2.416</v>
       </c>
       <c r="F144" s="0" t="n">
-        <v>3.793</v>
+        <v>5.442</v>
       </c>
       <c r="G144" s="0" t="n">
         <v>1.188</v>
@@ -4539,25 +4542,25 @@
         <v>151</v>
       </c>
       <c r="B145" s="0" t="n">
-        <v>2997.787</v>
+        <v>3067.38</v>
       </c>
       <c r="C145" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D145" s="0" t="n">
-        <v>43.729</v>
+        <v>44.069</v>
       </c>
       <c r="E145" s="0" t="n">
-        <v>2.256</v>
+        <v>2.416</v>
       </c>
       <c r="F145" s="0" t="n">
-        <v>3.793</v>
+        <v>5.442</v>
       </c>
       <c r="G145" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H145" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4565,25 +4568,25 @@
         <v>152</v>
       </c>
       <c r="B146" s="0" t="n">
-        <v>2997.787</v>
+        <v>3067.38</v>
       </c>
       <c r="C146" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D146" s="0" t="n">
-        <v>43.729</v>
+        <v>44.069</v>
       </c>
       <c r="E146" s="0" t="n">
-        <v>2.256</v>
+        <v>2.416</v>
       </c>
       <c r="F146" s="0" t="n">
-        <v>3.793</v>
+        <v>5.442</v>
       </c>
       <c r="G146" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H146" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4591,25 +4594,25 @@
         <v>153</v>
       </c>
       <c r="B147" s="0" t="n">
-        <v>2997.787</v>
+        <v>3067.856</v>
       </c>
       <c r="C147" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D147" s="0" t="n">
-        <v>43.729</v>
+        <v>44.069</v>
       </c>
       <c r="E147" s="0" t="n">
-        <v>2.256</v>
+        <v>2.416</v>
       </c>
       <c r="F147" s="0" t="n">
-        <v>3.793</v>
+        <v>5.442</v>
       </c>
       <c r="G147" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H147" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4617,25 +4620,25 @@
         <v>154</v>
       </c>
       <c r="B148" s="0" t="n">
-        <v>2997.787</v>
+        <v>3068.084</v>
       </c>
       <c r="C148" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D148" s="0" t="n">
-        <v>43.736</v>
+        <v>44.069</v>
       </c>
       <c r="E148" s="0" t="n">
-        <v>2.256</v>
+        <v>2.416</v>
       </c>
       <c r="F148" s="0" t="n">
-        <v>3.793</v>
+        <v>5.442</v>
       </c>
       <c r="G148" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H148" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4643,25 +4646,25 @@
         <v>155</v>
       </c>
       <c r="B149" s="0" t="n">
-        <v>2997.937</v>
+        <v>3068.314</v>
       </c>
       <c r="C149" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D149" s="0" t="n">
-        <v>43.736</v>
+        <v>44.069</v>
       </c>
       <c r="E149" s="0" t="n">
-        <v>2.256</v>
+        <v>2.416</v>
       </c>
       <c r="F149" s="0" t="n">
-        <v>3.793</v>
+        <v>5.442</v>
       </c>
       <c r="G149" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H149" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4669,25 +4672,25 @@
         <v>156</v>
       </c>
       <c r="B150" s="0" t="n">
-        <v>2997.937</v>
+        <v>3068.314</v>
       </c>
       <c r="C150" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D150" s="0" t="n">
-        <v>43.736</v>
+        <v>44.069</v>
       </c>
       <c r="E150" s="0" t="n">
-        <v>2.256</v>
+        <v>2.416</v>
       </c>
       <c r="F150" s="0" t="n">
-        <v>3.793</v>
+        <v>5.442</v>
       </c>
       <c r="G150" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H150" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4695,25 +4698,25 @@
         <v>157</v>
       </c>
       <c r="B151" s="0" t="n">
-        <v>2997.937</v>
+        <v>3068.314</v>
       </c>
       <c r="C151" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D151" s="0" t="n">
-        <v>43.736</v>
+        <v>44.069</v>
       </c>
       <c r="E151" s="0" t="n">
-        <v>2.256</v>
+        <v>2.416</v>
       </c>
       <c r="F151" s="0" t="n">
-        <v>4.549</v>
+        <v>5.69</v>
       </c>
       <c r="G151" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H151" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4721,25 +4724,25 @@
         <v>158</v>
       </c>
       <c r="B152" s="0" t="n">
-        <v>2997.937</v>
+        <v>3068.314</v>
       </c>
       <c r="C152" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D152" s="0" t="n">
-        <v>43.736</v>
+        <v>44.069</v>
       </c>
       <c r="E152" s="0" t="n">
-        <v>2.256</v>
+        <v>2.416</v>
       </c>
       <c r="F152" s="0" t="n">
-        <v>4.949</v>
+        <v>5.918</v>
       </c>
       <c r="G152" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H152" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4747,25 +4750,25 @@
         <v>159</v>
       </c>
       <c r="B153" s="0" t="n">
-        <v>2997.937</v>
+        <v>3068.314</v>
       </c>
       <c r="C153" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D153" s="0" t="n">
-        <v>43.736</v>
+        <v>44.069</v>
       </c>
       <c r="E153" s="0" t="n">
-        <v>2.256</v>
+        <v>2.416</v>
       </c>
       <c r="F153" s="0" t="n">
-        <v>4.949</v>
+        <v>5.918</v>
       </c>
       <c r="G153" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H153" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4773,25 +4776,25 @@
         <v>160</v>
       </c>
       <c r="B154" s="0" t="n">
-        <v>2997.937</v>
+        <v>3068.314</v>
       </c>
       <c r="C154" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D154" s="0" t="n">
-        <v>43.736</v>
+        <v>44.292</v>
       </c>
       <c r="E154" s="0" t="n">
-        <v>2.256</v>
+        <v>2.416</v>
       </c>
       <c r="F154" s="0" t="n">
-        <v>4.949</v>
+        <v>5.918</v>
       </c>
       <c r="G154" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H154" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4799,25 +4802,25 @@
         <v>161</v>
       </c>
       <c r="B155" s="0" t="n">
-        <v>2997.937</v>
+        <v>3075.872</v>
       </c>
       <c r="C155" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D155" s="0" t="n">
-        <v>43.736</v>
+        <v>44.292</v>
       </c>
       <c r="E155" s="0" t="n">
-        <v>2.256</v>
+        <v>2.416</v>
       </c>
       <c r="F155" s="0" t="n">
-        <v>4.949</v>
+        <v>5.918</v>
       </c>
       <c r="G155" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H155" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4825,25 +4828,25 @@
         <v>162</v>
       </c>
       <c r="B156" s="0" t="n">
-        <v>3005.43</v>
+        <v>3094.404</v>
       </c>
       <c r="C156" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D156" s="0" t="n">
-        <v>43.736</v>
+        <v>44.292</v>
       </c>
       <c r="E156" s="0" t="n">
-        <v>2.256</v>
+        <v>2.416</v>
       </c>
       <c r="F156" s="0" t="n">
-        <v>4.949</v>
+        <v>5.918</v>
       </c>
       <c r="G156" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H156" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4851,25 +4854,25 @@
         <v>163</v>
       </c>
       <c r="B157" s="0" t="n">
-        <v>3010.782</v>
+        <v>3094.404</v>
       </c>
       <c r="C157" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D157" s="0" t="n">
-        <v>43.736</v>
+        <v>44.292</v>
       </c>
       <c r="E157" s="0" t="n">
-        <v>2.256</v>
+        <v>2.416</v>
       </c>
       <c r="F157" s="0" t="n">
-        <v>4.949</v>
+        <v>5.918</v>
       </c>
       <c r="G157" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H157" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4877,25 +4880,25 @@
         <v>164</v>
       </c>
       <c r="B158" s="0" t="n">
-        <v>3010.782</v>
+        <v>3094.404</v>
       </c>
       <c r="C158" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D158" s="0" t="n">
-        <v>43.736</v>
+        <v>44.292</v>
       </c>
       <c r="E158" s="0" t="n">
-        <v>2.256</v>
+        <v>2.416</v>
       </c>
       <c r="F158" s="0" t="n">
-        <v>4.949</v>
+        <v>5.918</v>
       </c>
       <c r="G158" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H158" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4903,25 +4906,25 @@
         <v>165</v>
       </c>
       <c r="B159" s="0" t="n">
-        <v>3010.782</v>
+        <v>3094.404</v>
       </c>
       <c r="C159" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D159" s="0" t="n">
-        <v>43.971</v>
+        <v>44.292</v>
       </c>
       <c r="E159" s="0" t="n">
-        <v>2.256</v>
+        <v>2.416</v>
       </c>
       <c r="F159" s="0" t="n">
-        <v>4.949</v>
+        <v>5.918</v>
       </c>
       <c r="G159" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H159" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4929,25 +4932,25 @@
         <v>166</v>
       </c>
       <c r="B160" s="0" t="n">
-        <v>3010.782</v>
+        <v>3104.759</v>
       </c>
       <c r="C160" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D160" s="0" t="n">
-        <v>43.971</v>
+        <v>44.292</v>
       </c>
       <c r="E160" s="0" t="n">
-        <v>2.256</v>
+        <v>2.416</v>
       </c>
       <c r="F160" s="0" t="n">
-        <v>5.216</v>
+        <v>5.918</v>
       </c>
       <c r="G160" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H160" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4955,25 +4958,25 @@
         <v>167</v>
       </c>
       <c r="B161" s="0" t="n">
-        <v>3010.782</v>
+        <v>3104.759</v>
       </c>
       <c r="C161" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D161" s="0" t="n">
-        <v>43.971</v>
+        <v>44.292</v>
       </c>
       <c r="E161" s="0" t="n">
-        <v>2.256</v>
+        <v>2.416</v>
       </c>
       <c r="F161" s="0" t="n">
-        <v>5.442</v>
+        <v>5.918</v>
       </c>
       <c r="G161" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H161" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4981,25 +4984,25 @@
         <v>168</v>
       </c>
       <c r="B162" s="0" t="n">
-        <v>3010.782</v>
+        <v>3104.759</v>
       </c>
       <c r="C162" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D162" s="0" t="n">
-        <v>43.971</v>
+        <v>44.292</v>
       </c>
       <c r="E162" s="0" t="n">
-        <v>2.362</v>
+        <v>2.416</v>
       </c>
       <c r="F162" s="0" t="n">
-        <v>5.442</v>
+        <v>5.918</v>
       </c>
       <c r="G162" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H162" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5007,25 +5010,25 @@
         <v>169</v>
       </c>
       <c r="B163" s="0" t="n">
-        <v>3018.213</v>
+        <v>3104.759</v>
       </c>
       <c r="C163" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D163" s="0" t="n">
-        <v>43.971</v>
+        <v>44.292</v>
       </c>
       <c r="E163" s="0" t="n">
-        <v>2.362</v>
+        <v>2.416</v>
       </c>
       <c r="F163" s="0" t="n">
-        <v>5.442</v>
+        <v>5.918</v>
       </c>
       <c r="G163" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H163" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5033,25 +5036,25 @@
         <v>170</v>
       </c>
       <c r="B164" s="0" t="n">
-        <v>3027.483</v>
+        <v>3104.759</v>
       </c>
       <c r="C164" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D164" s="0" t="n">
-        <v>43.971</v>
+        <v>44.292</v>
       </c>
       <c r="E164" s="0" t="n">
-        <v>2.362</v>
+        <v>2.416</v>
       </c>
       <c r="F164" s="0" t="n">
-        <v>5.442</v>
+        <v>5.918</v>
       </c>
       <c r="G164" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H164" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5059,25 +5062,25 @@
         <v>171</v>
       </c>
       <c r="B165" s="0" t="n">
-        <v>3037.77</v>
+        <v>3104.759</v>
       </c>
       <c r="C165" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D165" s="0" t="n">
-        <v>43.971</v>
+        <v>44.292</v>
       </c>
       <c r="E165" s="0" t="n">
-        <v>2.362</v>
+        <v>2.416</v>
       </c>
       <c r="F165" s="0" t="n">
-        <v>5.442</v>
+        <v>5.918</v>
       </c>
       <c r="G165" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H165" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5085,25 +5088,25 @@
         <v>172</v>
       </c>
       <c r="B166" s="0" t="n">
-        <v>3037.77</v>
+        <v>3104.759</v>
       </c>
       <c r="C166" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D166" s="0" t="n">
-        <v>43.971</v>
+        <v>44.292</v>
       </c>
       <c r="E166" s="0" t="n">
-        <v>2.362</v>
+        <v>2.416</v>
       </c>
       <c r="F166" s="0" t="n">
-        <v>5.442</v>
+        <v>5.918</v>
       </c>
       <c r="G166" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H166" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5111,25 +5114,25 @@
         <v>173</v>
       </c>
       <c r="B167" s="0" t="n">
-        <v>3037.77</v>
+        <v>3104.759</v>
       </c>
       <c r="C167" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D167" s="0" t="n">
-        <v>43.971</v>
+        <v>44.292</v>
       </c>
       <c r="E167" s="0" t="n">
-        <v>2.362</v>
+        <v>2.416</v>
       </c>
       <c r="F167" s="0" t="n">
-        <v>5.442</v>
+        <v>5.918</v>
       </c>
       <c r="G167" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H167" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5137,25 +5140,25 @@
         <v>174</v>
       </c>
       <c r="B168" s="0" t="n">
-        <v>3037.77</v>
+        <v>3104.786</v>
       </c>
       <c r="C168" s="0" t="n">
-        <v>164.049</v>
+        <v>164.093</v>
       </c>
       <c r="D168" s="0" t="n">
-        <v>43.979</v>
+        <v>44.292</v>
       </c>
       <c r="E168" s="0" t="n">
-        <v>2.362</v>
+        <v>2.416</v>
       </c>
       <c r="F168" s="0" t="n">
-        <v>5.442</v>
+        <v>5.918</v>
       </c>
       <c r="G168" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H168" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5163,25 +5166,25 @@
         <v>175</v>
       </c>
       <c r="B169" s="0" t="n">
-        <v>3045.333</v>
+        <v>3104.798</v>
       </c>
       <c r="C169" s="0" t="n">
-        <v>164.049</v>
+        <v>164.093</v>
       </c>
       <c r="D169" s="0" t="n">
-        <v>43.979</v>
+        <v>44.292</v>
       </c>
       <c r="E169" s="0" t="n">
-        <v>2.362</v>
+        <v>2.416</v>
       </c>
       <c r="F169" s="0" t="n">
-        <v>5.442</v>
+        <v>5.918</v>
       </c>
       <c r="G169" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H169" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5189,25 +5192,25 @@
         <v>176</v>
       </c>
       <c r="B170" s="0" t="n">
-        <v>3067.38</v>
+        <v>3104.798</v>
       </c>
       <c r="C170" s="0" t="n">
-        <v>164.049</v>
+        <v>164.093</v>
       </c>
       <c r="D170" s="0" t="n">
-        <v>43.979</v>
+        <v>44.292</v>
       </c>
       <c r="E170" s="0" t="n">
-        <v>2.362</v>
+        <v>2.416</v>
       </c>
       <c r="F170" s="0" t="n">
-        <v>5.442</v>
+        <v>5.918</v>
       </c>
       <c r="G170" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H170" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5215,25 +5218,25 @@
         <v>177</v>
       </c>
       <c r="B171" s="0" t="n">
-        <v>3067.38</v>
+        <v>3104.798</v>
       </c>
       <c r="C171" s="0" t="n">
-        <v>164.049</v>
+        <v>164.093</v>
       </c>
       <c r="D171" s="0" t="n">
-        <v>44.017</v>
+        <v>44.292</v>
       </c>
       <c r="E171" s="0" t="n">
         <v>2.416</v>
       </c>
       <c r="F171" s="0" t="n">
-        <v>5.442</v>
+        <v>5.918</v>
       </c>
       <c r="G171" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H171" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5241,19 +5244,19 @@
         <v>178</v>
       </c>
       <c r="B172" s="0" t="n">
-        <v>3067.38</v>
+        <v>3104.798</v>
       </c>
       <c r="C172" s="0" t="n">
-        <v>164.049</v>
+        <v>164.093</v>
       </c>
       <c r="D172" s="0" t="n">
-        <v>44.069</v>
+        <v>44.292</v>
       </c>
       <c r="E172" s="0" t="n">
         <v>2.416</v>
       </c>
       <c r="F172" s="0" t="n">
-        <v>5.442</v>
+        <v>5.918</v>
       </c>
       <c r="G172" s="0" t="n">
         <v>1.188</v>
@@ -5267,19 +5270,19 @@
         <v>179</v>
       </c>
       <c r="B173" s="0" t="n">
-        <v>3067.38</v>
+        <v>3104.798</v>
       </c>
       <c r="C173" s="0" t="n">
-        <v>164.049</v>
+        <v>164.093</v>
       </c>
       <c r="D173" s="0" t="n">
-        <v>44.069</v>
+        <v>44.292</v>
       </c>
       <c r="E173" s="0" t="n">
         <v>2.416</v>
       </c>
       <c r="F173" s="0" t="n">
-        <v>5.442</v>
+        <v>5.918</v>
       </c>
       <c r="G173" s="0" t="n">
         <v>1.188</v>
@@ -5293,19 +5296,19 @@
         <v>180</v>
       </c>
       <c r="B174" s="0" t="n">
-        <v>3067.856</v>
+        <v>3104.798</v>
       </c>
       <c r="C174" s="0" t="n">
-        <v>164.049</v>
+        <v>164.093</v>
       </c>
       <c r="D174" s="0" t="n">
-        <v>44.069</v>
+        <v>44.292</v>
       </c>
       <c r="E174" s="0" t="n">
         <v>2.416</v>
       </c>
       <c r="F174" s="0" t="n">
-        <v>5.442</v>
+        <v>5.918</v>
       </c>
       <c r="G174" s="0" t="n">
         <v>1.188</v>
@@ -5319,19 +5322,19 @@
         <v>181</v>
       </c>
       <c r="B175" s="0" t="n">
-        <v>3068.084</v>
+        <v>3104.798</v>
       </c>
       <c r="C175" s="0" t="n">
-        <v>164.049</v>
+        <v>164.093</v>
       </c>
       <c r="D175" s="0" t="n">
-        <v>44.069</v>
+        <v>44.292</v>
       </c>
       <c r="E175" s="0" t="n">
         <v>2.416</v>
       </c>
       <c r="F175" s="0" t="n">
-        <v>5.442</v>
+        <v>5.918</v>
       </c>
       <c r="G175" s="0" t="n">
         <v>1.188</v>
@@ -5345,19 +5348,19 @@
         <v>182</v>
       </c>
       <c r="B176" s="0" t="n">
-        <v>3068.314</v>
+        <v>3104.798</v>
       </c>
       <c r="C176" s="0" t="n">
-        <v>164.049</v>
+        <v>164.093</v>
       </c>
       <c r="D176" s="0" t="n">
-        <v>44.069</v>
+        <v>44.292</v>
       </c>
       <c r="E176" s="0" t="n">
         <v>2.416</v>
       </c>
       <c r="F176" s="0" t="n">
-        <v>5.442</v>
+        <v>5.918</v>
       </c>
       <c r="G176" s="0" t="n">
         <v>1.188</v>
@@ -5371,19 +5374,19 @@
         <v>183</v>
       </c>
       <c r="B177" s="0" t="n">
-        <v>3068.314</v>
+        <v>3104.798</v>
       </c>
       <c r="C177" s="0" t="n">
-        <v>164.049</v>
+        <v>164.093</v>
       </c>
       <c r="D177" s="0" t="n">
-        <v>44.069</v>
+        <v>44.292</v>
       </c>
       <c r="E177" s="0" t="n">
         <v>2.416</v>
       </c>
       <c r="F177" s="0" t="n">
-        <v>5.442</v>
+        <v>5.918</v>
       </c>
       <c r="G177" s="0" t="n">
         <v>1.188</v>
@@ -5397,19 +5400,19 @@
         <v>184</v>
       </c>
       <c r="B178" s="0" t="n">
-        <v>3068.314</v>
+        <v>3104.798</v>
       </c>
       <c r="C178" s="0" t="n">
-        <v>164.049</v>
+        <v>164.093</v>
       </c>
       <c r="D178" s="0" t="n">
-        <v>44.069</v>
+        <v>44.292</v>
       </c>
       <c r="E178" s="0" t="n">
         <v>2.416</v>
       </c>
       <c r="F178" s="0" t="n">
-        <v>5.69</v>
+        <v>5.918</v>
       </c>
       <c r="G178" s="0" t="n">
         <v>1.188</v>
@@ -5423,13 +5426,13 @@
         <v>185</v>
       </c>
       <c r="B179" s="0" t="n">
-        <v>3068.314</v>
+        <v>3104.798</v>
       </c>
       <c r="C179" s="0" t="n">
-        <v>164.049</v>
+        <v>164.093</v>
       </c>
       <c r="D179" s="0" t="n">
-        <v>44.069</v>
+        <v>44.292</v>
       </c>
       <c r="E179" s="0" t="n">
         <v>2.416</v>
@@ -5449,13 +5452,13 @@
         <v>186</v>
       </c>
       <c r="B180" s="0" t="n">
-        <v>3068.314</v>
+        <v>3104.798</v>
       </c>
       <c r="C180" s="0" t="n">
-        <v>164.049</v>
+        <v>164.093</v>
       </c>
       <c r="D180" s="0" t="n">
-        <v>44.069</v>
+        <v>44.292</v>
       </c>
       <c r="E180" s="0" t="n">
         <v>2.416</v>
@@ -5475,10 +5478,10 @@
         <v>187</v>
       </c>
       <c r="B181" s="0" t="n">
-        <v>3068.314</v>
+        <v>3104.798</v>
       </c>
       <c r="C181" s="0" t="n">
-        <v>164.049</v>
+        <v>164.093</v>
       </c>
       <c r="D181" s="0" t="n">
         <v>44.292</v>
@@ -5501,10 +5504,10 @@
         <v>188</v>
       </c>
       <c r="B182" s="0" t="n">
-        <v>3075.872</v>
+        <v>3104.798</v>
       </c>
       <c r="C182" s="0" t="n">
-        <v>164.049</v>
+        <v>164.093</v>
       </c>
       <c r="D182" s="0" t="n">
         <v>44.292</v>
@@ -5527,10 +5530,10 @@
         <v>189</v>
       </c>
       <c r="B183" s="0" t="n">
-        <v>3094.404</v>
+        <v>3104.798</v>
       </c>
       <c r="C183" s="0" t="n">
-        <v>164.049</v>
+        <v>164.203</v>
       </c>
       <c r="D183" s="0" t="n">
         <v>44.292</v>
@@ -5553,10 +5556,10 @@
         <v>190</v>
       </c>
       <c r="B184" s="0" t="n">
-        <v>3094.404</v>
+        <v>3104.798</v>
       </c>
       <c r="C184" s="0" t="n">
-        <v>164.049</v>
+        <v>164.203</v>
       </c>
       <c r="D184" s="0" t="n">
         <v>44.292</v>
@@ -5579,10 +5582,10 @@
         <v>191</v>
       </c>
       <c r="B185" s="0" t="n">
-        <v>3094.404</v>
+        <v>3104.798</v>
       </c>
       <c r="C185" s="0" t="n">
-        <v>164.049</v>
+        <v>164.203</v>
       </c>
       <c r="D185" s="0" t="n">
         <v>44.292</v>
@@ -5605,10 +5608,10 @@
         <v>192</v>
       </c>
       <c r="B186" s="0" t="n">
-        <v>3094.404</v>
+        <v>3104.798</v>
       </c>
       <c r="C186" s="0" t="n">
-        <v>164.049</v>
+        <v>164.203</v>
       </c>
       <c r="D186" s="0" t="n">
         <v>44.292</v>
@@ -5631,10 +5634,10 @@
         <v>193</v>
       </c>
       <c r="B187" s="0" t="n">
-        <v>3104.759</v>
+        <v>3104.798</v>
       </c>
       <c r="C187" s="0" t="n">
-        <v>164.049</v>
+        <v>164.203</v>
       </c>
       <c r="D187" s="0" t="n">
         <v>44.292</v>
@@ -5657,10 +5660,10 @@
         <v>194</v>
       </c>
       <c r="B188" s="0" t="n">
-        <v>3104.759</v>
+        <v>3104.798</v>
       </c>
       <c r="C188" s="0" t="n">
-        <v>164.049</v>
+        <v>164.203</v>
       </c>
       <c r="D188" s="0" t="n">
         <v>44.292</v>
@@ -5683,10 +5686,10 @@
         <v>195</v>
       </c>
       <c r="B189" s="0" t="n">
-        <v>3104.759</v>
+        <v>3104.808</v>
       </c>
       <c r="C189" s="0" t="n">
-        <v>164.049</v>
+        <v>164.247</v>
       </c>
       <c r="D189" s="0" t="n">
         <v>44.292</v>
@@ -5709,10 +5712,10 @@
         <v>196</v>
       </c>
       <c r="B190" s="0" t="n">
-        <v>3104.759</v>
+        <v>3104.808</v>
       </c>
       <c r="C190" s="0" t="n">
-        <v>164.049</v>
+        <v>164.247</v>
       </c>
       <c r="D190" s="0" t="n">
         <v>44.292</v>
@@ -5735,10 +5738,10 @@
         <v>197</v>
       </c>
       <c r="B191" s="0" t="n">
-        <v>3104.759</v>
+        <v>3104.808</v>
       </c>
       <c r="C191" s="0" t="n">
-        <v>164.049</v>
+        <v>164.247</v>
       </c>
       <c r="D191" s="0" t="n">
         <v>44.292</v>
@@ -5761,10 +5764,10 @@
         <v>198</v>
       </c>
       <c r="B192" s="0" t="n">
-        <v>3104.759</v>
+        <v>3104.808</v>
       </c>
       <c r="C192" s="0" t="n">
-        <v>164.049</v>
+        <v>164.247</v>
       </c>
       <c r="D192" s="0" t="n">
         <v>44.292</v>
@@ -5787,10 +5790,10 @@
         <v>199</v>
       </c>
       <c r="B193" s="0" t="n">
-        <v>3104.759</v>
+        <v>3104.808</v>
       </c>
       <c r="C193" s="0" t="n">
-        <v>164.049</v>
+        <v>164.247</v>
       </c>
       <c r="D193" s="0" t="n">
         <v>44.292</v>
@@ -5813,10 +5816,10 @@
         <v>200</v>
       </c>
       <c r="B194" s="0" t="n">
-        <v>3104.759</v>
+        <v>3104.808</v>
       </c>
       <c r="C194" s="0" t="n">
-        <v>164.049</v>
+        <v>164.247</v>
       </c>
       <c r="D194" s="0" t="n">
         <v>44.292</v>
@@ -5839,10 +5842,10 @@
         <v>201</v>
       </c>
       <c r="B195" s="0" t="n">
-        <v>3104.786</v>
+        <v>3104.808</v>
       </c>
       <c r="C195" s="0" t="n">
-        <v>164.093</v>
+        <v>164.247</v>
       </c>
       <c r="D195" s="0" t="n">
         <v>44.292</v>
@@ -5865,10 +5868,10 @@
         <v>202</v>
       </c>
       <c r="B196" s="0" t="n">
-        <v>3104.798</v>
+        <v>3104.808</v>
       </c>
       <c r="C196" s="0" t="n">
-        <v>164.093</v>
+        <v>164.247</v>
       </c>
       <c r="D196" s="0" t="n">
         <v>44.292</v>
@@ -5891,10 +5894,10 @@
         <v>203</v>
       </c>
       <c r="B197" s="0" t="n">
-        <v>3104.798</v>
+        <v>3104.808</v>
       </c>
       <c r="C197" s="0" t="n">
-        <v>164.093</v>
+        <v>164.249</v>
       </c>
       <c r="D197" s="0" t="n">
         <v>44.292</v>
@@ -5917,10 +5920,10 @@
         <v>204</v>
       </c>
       <c r="B198" s="0" t="n">
-        <v>3104.798</v>
+        <v>3104.808</v>
       </c>
       <c r="C198" s="0" t="n">
-        <v>164.093</v>
+        <v>164.249</v>
       </c>
       <c r="D198" s="0" t="n">
         <v>44.292</v>
@@ -5943,10 +5946,10 @@
         <v>205</v>
       </c>
       <c r="B199" s="0" t="n">
-        <v>3104.798</v>
+        <v>3104.808</v>
       </c>
       <c r="C199" s="0" t="n">
-        <v>164.093</v>
+        <v>164.249</v>
       </c>
       <c r="D199" s="0" t="n">
         <v>44.292</v>
@@ -5969,10 +5972,10 @@
         <v>206</v>
       </c>
       <c r="B200" s="0" t="n">
-        <v>3104.798</v>
+        <v>3104.808</v>
       </c>
       <c r="C200" s="0" t="n">
-        <v>164.093</v>
+        <v>164.249</v>
       </c>
       <c r="D200" s="0" t="n">
         <v>44.292</v>
@@ -5995,10 +5998,10 @@
         <v>207</v>
       </c>
       <c r="B201" s="0" t="n">
-        <v>3104.798</v>
+        <v>3104.808</v>
       </c>
       <c r="C201" s="0" t="n">
-        <v>164.093</v>
+        <v>164.249</v>
       </c>
       <c r="D201" s="0" t="n">
         <v>44.292</v>
@@ -6021,10 +6024,10 @@
         <v>208</v>
       </c>
       <c r="B202" s="0" t="n">
-        <v>3104.798</v>
+        <v>3104.808</v>
       </c>
       <c r="C202" s="0" t="n">
-        <v>164.093</v>
+        <v>164.249</v>
       </c>
       <c r="D202" s="0" t="n">
         <v>44.292</v>
@@ -6047,10 +6050,10 @@
         <v>209</v>
       </c>
       <c r="B203" s="0" t="n">
-        <v>3104.798</v>
+        <v>3104.808</v>
       </c>
       <c r="C203" s="0" t="n">
-        <v>164.093</v>
+        <v>164.249</v>
       </c>
       <c r="D203" s="0" t="n">
         <v>44.292</v>
@@ -6073,10 +6076,10 @@
         <v>210</v>
       </c>
       <c r="B204" s="0" t="n">
-        <v>3104.798</v>
+        <v>3104.808</v>
       </c>
       <c r="C204" s="0" t="n">
-        <v>164.093</v>
+        <v>164.249</v>
       </c>
       <c r="D204" s="0" t="n">
         <v>44.292</v>
@@ -6099,10 +6102,10 @@
         <v>211</v>
       </c>
       <c r="B205" s="0" t="n">
-        <v>3104.798</v>
+        <v>3104.808</v>
       </c>
       <c r="C205" s="0" t="n">
-        <v>164.093</v>
+        <v>164.249</v>
       </c>
       <c r="D205" s="0" t="n">
         <v>44.292</v>
@@ -6125,10 +6128,10 @@
         <v>212</v>
       </c>
       <c r="B206" s="0" t="n">
-        <v>3104.798</v>
+        <v>3104.808</v>
       </c>
       <c r="C206" s="0" t="n">
-        <v>164.093</v>
+        <v>164.249</v>
       </c>
       <c r="D206" s="0" t="n">
         <v>44.292</v>
@@ -6151,10 +6154,10 @@
         <v>213</v>
       </c>
       <c r="B207" s="0" t="n">
-        <v>3104.798</v>
+        <v>3104.808</v>
       </c>
       <c r="C207" s="0" t="n">
-        <v>164.093</v>
+        <v>164.249</v>
       </c>
       <c r="D207" s="0" t="n">
         <v>44.292</v>
@@ -6177,10 +6180,10 @@
         <v>214</v>
       </c>
       <c r="B208" s="0" t="n">
-        <v>3104.798</v>
+        <v>3104.808</v>
       </c>
       <c r="C208" s="0" t="n">
-        <v>164.093</v>
+        <v>164.249</v>
       </c>
       <c r="D208" s="0" t="n">
         <v>44.292</v>
@@ -6203,10 +6206,10 @@
         <v>215</v>
       </c>
       <c r="B209" s="0" t="n">
-        <v>3104.798</v>
+        <v>3104.808</v>
       </c>
       <c r="C209" s="0" t="n">
-        <v>164.093</v>
+        <v>164.249</v>
       </c>
       <c r="D209" s="0" t="n">
         <v>44.292</v>
@@ -6229,10 +6232,10 @@
         <v>216</v>
       </c>
       <c r="B210" s="0" t="n">
-        <v>3104.798</v>
+        <v>3104.808</v>
       </c>
       <c r="C210" s="0" t="n">
-        <v>164.203</v>
+        <v>164.249</v>
       </c>
       <c r="D210" s="0" t="n">
         <v>44.292</v>
@@ -6255,10 +6258,10 @@
         <v>217</v>
       </c>
       <c r="B211" s="0" t="n">
-        <v>3104.798</v>
+        <v>3104.808</v>
       </c>
       <c r="C211" s="0" t="n">
-        <v>164.203</v>
+        <v>164.249</v>
       </c>
       <c r="D211" s="0" t="n">
         <v>44.292</v>
@@ -6273,6 +6276,32 @@
         <v>1.188</v>
       </c>
       <c r="H211" s="0" t="n">
+        <v>1924.316</v>
+      </c>
+    </row>
+    <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A212" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="B212" s="0" t="n">
+        <v>3119.148</v>
+      </c>
+      <c r="C212" s="0" t="n">
+        <v>182.007</v>
+      </c>
+      <c r="D212" s="0" t="n">
+        <v>44.292</v>
+      </c>
+      <c r="E212" s="0" t="n">
+        <v>2.416</v>
+      </c>
+      <c r="F212" s="0" t="n">
+        <v>5.918</v>
+      </c>
+      <c r="G212" s="0" t="n">
+        <v>1.188</v>
+      </c>
+      <c r="H212" s="0" t="n">
         <v>1924.316</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Mise à jour index
</commit_message>
<xml_diff>
--- a/rapport_compteur.xlsx
+++ b/rapport_compteur.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="217">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -46,90 +46,6 @@
     <t xml:space="preserve">Inconnu</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-09-10 23:30:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-09-11 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-09-12 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-09-13 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-09-14 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-09-15 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-09-16 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-09-17 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-09-18 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-09-19 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-09-20 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-09-21 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-09-22 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-09-23 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-09-24 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-09-25 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-09-26 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-09-27 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-09-28 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-09-29 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-09-30 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-10-01 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-10-02 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-10-03 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-10-04 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-10-05 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-10-06 00:00:00 +0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-10-07 00:00:00 +0200</t>
-  </si>
-  <si>
     <t xml:space="preserve">2023-10-08 00:00:00 +0200</t>
   </si>
   <si>
@@ -676,7 +592,85 @@
     <t xml:space="preserve">2024-05-06 00:00:00 +0200</t>
   </si>
   <si>
-    <t xml:space="preserve">2024-05-06 19:05:54 +0200</t>
+    <t xml:space="preserve">2024-05-07 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-08 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-09 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-10 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-11 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-12 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-13 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-14 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-15 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-16 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-17 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-18 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-19 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-20 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-21 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-22 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-23 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-24 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-25 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-26 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-27 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-28 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-29 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-30 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-31 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-06-01 00:00:00 +0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-06-02 00:00:00 +0200</t>
   </si>
 </sst>
 </file>
@@ -777,10 +771,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H212"/>
+  <dimension ref="A1:H210"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
+      <selection pane="topLeft" activeCell="A210" activeCellId="0" sqref="A210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -824,10 +818,10 @@
         <v>8</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>2767.909</v>
+        <v>2842.772</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>145.165</v>
+        <v>157.472</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>41.965</v>
@@ -850,10 +844,10 @@
         <v>9</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>2767.917</v>
+        <v>2842.772</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>145.165</v>
+        <v>157.472</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>41.965</v>
@@ -876,10 +870,10 @@
         <v>10</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>2770.446</v>
+        <v>2842.772</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>151.112</v>
+        <v>157.472</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>41.965</v>
@@ -902,10 +896,10 @@
         <v>11</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>2770.446</v>
+        <v>2842.772</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>151.112</v>
+        <v>157.472</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>41.965</v>
@@ -928,10 +922,10 @@
         <v>12</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>2770.446</v>
+        <v>2842.772</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>151.112</v>
+        <v>157.472</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>41.965</v>
@@ -954,10 +948,10 @@
         <v>13</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>2770.446</v>
+        <v>2842.772</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>151.112</v>
+        <v>157.472</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>41.965</v>
@@ -980,10 +974,10 @@
         <v>14</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>2770.752</v>
+        <v>2842.772</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>151.112</v>
+        <v>157.472</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>41.965</v>
@@ -1006,10 +1000,10 @@
         <v>15</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>2770.752</v>
+        <v>2842.772</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>151.112</v>
+        <v>157.472</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>41.965</v>
@@ -1032,10 +1026,10 @@
         <v>16</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>2770.752</v>
+        <v>2843.983</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>151.112</v>
+        <v>157.472</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>41.965</v>
@@ -1058,10 +1052,10 @@
         <v>17</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>2771.824</v>
+        <v>2843.983</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>151.112</v>
+        <v>157.472</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>41.965</v>
@@ -1084,10 +1078,10 @@
         <v>18</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>2771.824</v>
+        <v>2843.983</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>151.112</v>
+        <v>157.472</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>41.965</v>
@@ -1110,10 +1104,10 @@
         <v>19</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>2771.951</v>
+        <v>2843.983</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>151.112</v>
+        <v>157.472</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>41.965</v>
@@ -1136,10 +1130,10 @@
         <v>20</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>2789.241</v>
+        <v>2843.983</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>151.112</v>
+        <v>157.472</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>41.965</v>
@@ -1162,10 +1156,10 @@
         <v>21</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>2811.081</v>
+        <v>2843.983</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>151.112</v>
+        <v>157.472</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>41.965</v>
@@ -1188,10 +1182,10 @@
         <v>22</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>2815.751</v>
+        <v>2845.039</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>151.112</v>
+        <v>157.472</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>41.965</v>
@@ -1214,7 +1208,7 @@
         <v>23</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>2838.684</v>
+        <v>2845.039</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>157.472</v>
@@ -1240,7 +1234,7 @@
         <v>24</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>2840.266</v>
+        <v>2845.039</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>157.472</v>
@@ -1266,7 +1260,7 @@
         <v>25</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>2840.531</v>
+        <v>2845.039</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>157.472</v>
@@ -1292,7 +1286,7 @@
         <v>26</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>2840.531</v>
+        <v>2845.039</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>157.472</v>
@@ -1318,7 +1312,7 @@
         <v>27</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>2840.843</v>
+        <v>2845.039</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>157.472</v>
@@ -1344,7 +1338,7 @@
         <v>28</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>2840.843</v>
+        <v>2845.039</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>157.472</v>
@@ -1370,7 +1364,7 @@
         <v>29</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>2840.843</v>
+        <v>2845.039</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>157.472</v>
@@ -1396,10 +1390,10 @@
         <v>30</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>2840.843</v>
+        <v>2862.022</v>
       </c>
       <c r="C24" s="0" t="n">
-        <v>157.472</v>
+        <v>157.518</v>
       </c>
       <c r="D24" s="0" t="n">
         <v>41.965</v>
@@ -1422,10 +1416,10 @@
         <v>31</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>2841.947</v>
+        <v>2862.034</v>
       </c>
       <c r="C25" s="0" t="n">
-        <v>157.472</v>
+        <v>157.619</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>41.965</v>
@@ -1448,10 +1442,10 @@
         <v>32</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>2841.947</v>
+        <v>2863.113</v>
       </c>
       <c r="C26" s="0" t="n">
-        <v>157.472</v>
+        <v>157.619</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>41.965</v>
@@ -1474,10 +1468,10 @@
         <v>33</v>
       </c>
       <c r="B27" s="0" t="n">
-        <v>2841.947</v>
+        <v>2863.113</v>
       </c>
       <c r="C27" s="0" t="n">
-        <v>157.472</v>
+        <v>157.619</v>
       </c>
       <c r="D27" s="0" t="n">
         <v>41.965</v>
@@ -1500,10 +1494,10 @@
         <v>34</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>2841.947</v>
+        <v>2863.113</v>
       </c>
       <c r="C28" s="0" t="n">
-        <v>157.472</v>
+        <v>157.619</v>
       </c>
       <c r="D28" s="0" t="n">
         <v>41.965</v>
@@ -1526,10 +1520,10 @@
         <v>35</v>
       </c>
       <c r="B29" s="0" t="n">
-        <v>2842.039</v>
+        <v>2863.113</v>
       </c>
       <c r="C29" s="0" t="n">
-        <v>157.472</v>
+        <v>157.619</v>
       </c>
       <c r="D29" s="0" t="n">
         <v>41.965</v>
@@ -1552,10 +1546,10 @@
         <v>36</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>2842.772</v>
+        <v>2863.331</v>
       </c>
       <c r="C30" s="0" t="n">
-        <v>157.472</v>
+        <v>157.619</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>41.965</v>
@@ -1578,10 +1572,10 @@
         <v>37</v>
       </c>
       <c r="B31" s="0" t="n">
-        <v>2842.772</v>
+        <v>2863.721</v>
       </c>
       <c r="C31" s="0" t="n">
-        <v>157.472</v>
+        <v>157.619</v>
       </c>
       <c r="D31" s="0" t="n">
         <v>41.965</v>
@@ -1604,10 +1598,10 @@
         <v>38</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>2842.772</v>
+        <v>2863.721</v>
       </c>
       <c r="C32" s="0" t="n">
-        <v>157.472</v>
+        <v>157.619</v>
       </c>
       <c r="D32" s="0" t="n">
         <v>41.965</v>
@@ -1630,10 +1624,10 @@
         <v>39</v>
       </c>
       <c r="B33" s="0" t="n">
-        <v>2842.772</v>
+        <v>2864.183</v>
       </c>
       <c r="C33" s="0" t="n">
-        <v>157.472</v>
+        <v>157.619</v>
       </c>
       <c r="D33" s="0" t="n">
         <v>41.965</v>
@@ -1656,10 +1650,10 @@
         <v>40</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>2842.772</v>
+        <v>2864.183</v>
       </c>
       <c r="C34" s="0" t="n">
-        <v>157.472</v>
+        <v>157.619</v>
       </c>
       <c r="D34" s="0" t="n">
         <v>41.965</v>
@@ -1682,10 +1676,10 @@
         <v>41</v>
       </c>
       <c r="B35" s="0" t="n">
-        <v>2842.772</v>
+        <v>2864.404</v>
       </c>
       <c r="C35" s="0" t="n">
-        <v>157.472</v>
+        <v>157.619</v>
       </c>
       <c r="D35" s="0" t="n">
         <v>41.965</v>
@@ -1708,10 +1702,10 @@
         <v>42</v>
       </c>
       <c r="B36" s="0" t="n">
-        <v>2842.772</v>
+        <v>2864.404</v>
       </c>
       <c r="C36" s="0" t="n">
-        <v>157.472</v>
+        <v>157.619</v>
       </c>
       <c r="D36" s="0" t="n">
         <v>41.965</v>
@@ -1734,10 +1728,10 @@
         <v>43</v>
       </c>
       <c r="B37" s="0" t="n">
-        <v>2842.772</v>
+        <v>2875.844</v>
       </c>
       <c r="C37" s="0" t="n">
-        <v>157.472</v>
+        <v>157.619</v>
       </c>
       <c r="D37" s="0" t="n">
         <v>41.965</v>
@@ -1760,10 +1754,10 @@
         <v>44</v>
       </c>
       <c r="B38" s="0" t="n">
-        <v>2843.983</v>
+        <v>2875.844</v>
       </c>
       <c r="C38" s="0" t="n">
-        <v>157.472</v>
+        <v>157.619</v>
       </c>
       <c r="D38" s="0" t="n">
         <v>41.965</v>
@@ -1786,10 +1780,10 @@
         <v>45</v>
       </c>
       <c r="B39" s="0" t="n">
-        <v>2843.983</v>
+        <v>2875.844</v>
       </c>
       <c r="C39" s="0" t="n">
-        <v>157.472</v>
+        <v>157.619</v>
       </c>
       <c r="D39" s="0" t="n">
         <v>41.965</v>
@@ -1812,10 +1806,10 @@
         <v>46</v>
       </c>
       <c r="B40" s="0" t="n">
-        <v>2843.983</v>
+        <v>2875.844</v>
       </c>
       <c r="C40" s="0" t="n">
-        <v>157.472</v>
+        <v>157.619</v>
       </c>
       <c r="D40" s="0" t="n">
         <v>41.965</v>
@@ -1838,10 +1832,10 @@
         <v>47</v>
       </c>
       <c r="B41" s="0" t="n">
-        <v>2843.983</v>
+        <v>2875.853</v>
       </c>
       <c r="C41" s="0" t="n">
-        <v>157.472</v>
+        <v>157.619</v>
       </c>
       <c r="D41" s="0" t="n">
         <v>41.965</v>
@@ -1864,10 +1858,10 @@
         <v>48</v>
       </c>
       <c r="B42" s="0" t="n">
-        <v>2843.983</v>
+        <v>2876.161</v>
       </c>
       <c r="C42" s="0" t="n">
-        <v>157.472</v>
+        <v>157.619</v>
       </c>
       <c r="D42" s="0" t="n">
         <v>41.965</v>
@@ -1890,10 +1884,10 @@
         <v>49</v>
       </c>
       <c r="B43" s="0" t="n">
-        <v>2843.983</v>
+        <v>2876.161</v>
       </c>
       <c r="C43" s="0" t="n">
-        <v>157.472</v>
+        <v>157.619</v>
       </c>
       <c r="D43" s="0" t="n">
         <v>41.965</v>
@@ -1916,10 +1910,10 @@
         <v>50</v>
       </c>
       <c r="B44" s="0" t="n">
-        <v>2845.039</v>
+        <v>2876.397</v>
       </c>
       <c r="C44" s="0" t="n">
-        <v>157.472</v>
+        <v>157.619</v>
       </c>
       <c r="D44" s="0" t="n">
         <v>41.965</v>
@@ -1942,10 +1936,10 @@
         <v>51</v>
       </c>
       <c r="B45" s="0" t="n">
-        <v>2845.039</v>
+        <v>2886.936</v>
       </c>
       <c r="C45" s="0" t="n">
-        <v>157.472</v>
+        <v>157.782</v>
       </c>
       <c r="D45" s="0" t="n">
         <v>41.965</v>
@@ -1968,10 +1962,10 @@
         <v>52</v>
       </c>
       <c r="B46" s="0" t="n">
-        <v>2845.039</v>
+        <v>2887.492</v>
       </c>
       <c r="C46" s="0" t="n">
-        <v>157.472</v>
+        <v>157.782</v>
       </c>
       <c r="D46" s="0" t="n">
         <v>41.965</v>
@@ -1994,10 +1988,10 @@
         <v>53</v>
       </c>
       <c r="B47" s="0" t="n">
-        <v>2845.039</v>
+        <v>2887.771</v>
       </c>
       <c r="C47" s="0" t="n">
-        <v>157.472</v>
+        <v>157.782</v>
       </c>
       <c r="D47" s="0" t="n">
         <v>41.965</v>
@@ -2020,10 +2014,10 @@
         <v>54</v>
       </c>
       <c r="B48" s="0" t="n">
-        <v>2845.039</v>
+        <v>2887.771</v>
       </c>
       <c r="C48" s="0" t="n">
-        <v>157.472</v>
+        <v>157.782</v>
       </c>
       <c r="D48" s="0" t="n">
         <v>41.965</v>
@@ -2046,10 +2040,10 @@
         <v>55</v>
       </c>
       <c r="B49" s="0" t="n">
-        <v>2845.039</v>
+        <v>2887.771</v>
       </c>
       <c r="C49" s="0" t="n">
-        <v>157.472</v>
+        <v>157.782</v>
       </c>
       <c r="D49" s="0" t="n">
         <v>41.965</v>
@@ -2072,10 +2066,10 @@
         <v>56</v>
       </c>
       <c r="B50" s="0" t="n">
-        <v>2845.039</v>
+        <v>2888</v>
       </c>
       <c r="C50" s="0" t="n">
-        <v>157.472</v>
+        <v>157.782</v>
       </c>
       <c r="D50" s="0" t="n">
         <v>41.965</v>
@@ -2098,10 +2092,10 @@
         <v>57</v>
       </c>
       <c r="B51" s="0" t="n">
-        <v>2845.039</v>
+        <v>2888</v>
       </c>
       <c r="C51" s="0" t="n">
-        <v>157.472</v>
+        <v>157.782</v>
       </c>
       <c r="D51" s="0" t="n">
         <v>41.965</v>
@@ -2124,10 +2118,10 @@
         <v>58</v>
       </c>
       <c r="B52" s="0" t="n">
-        <v>2862.022</v>
+        <v>2899.866</v>
       </c>
       <c r="C52" s="0" t="n">
-        <v>157.518</v>
+        <v>157.782</v>
       </c>
       <c r="D52" s="0" t="n">
         <v>41.965</v>
@@ -2150,10 +2144,10 @@
         <v>59</v>
       </c>
       <c r="B53" s="0" t="n">
-        <v>2862.034</v>
+        <v>2899.866</v>
       </c>
       <c r="C53" s="0" t="n">
-        <v>157.619</v>
+        <v>157.782</v>
       </c>
       <c r="D53" s="0" t="n">
         <v>41.965</v>
@@ -2176,10 +2170,10 @@
         <v>60</v>
       </c>
       <c r="B54" s="0" t="n">
-        <v>2863.113</v>
+        <v>2899.866</v>
       </c>
       <c r="C54" s="0" t="n">
-        <v>157.619</v>
+        <v>157.782</v>
       </c>
       <c r="D54" s="0" t="n">
         <v>41.965</v>
@@ -2202,10 +2196,10 @@
         <v>61</v>
       </c>
       <c r="B55" s="0" t="n">
-        <v>2863.113</v>
+        <v>2899.866</v>
       </c>
       <c r="C55" s="0" t="n">
-        <v>157.619</v>
+        <v>157.782</v>
       </c>
       <c r="D55" s="0" t="n">
         <v>41.965</v>
@@ -2228,10 +2222,10 @@
         <v>62</v>
       </c>
       <c r="B56" s="0" t="n">
-        <v>2863.113</v>
+        <v>2899.866</v>
       </c>
       <c r="C56" s="0" t="n">
-        <v>157.619</v>
+        <v>157.782</v>
       </c>
       <c r="D56" s="0" t="n">
         <v>41.965</v>
@@ -2240,7 +2234,7 @@
         <v>2.256</v>
       </c>
       <c r="F56" s="0" t="n">
-        <v>2.942</v>
+        <v>3.311</v>
       </c>
       <c r="G56" s="0" t="n">
         <v>1.188</v>
@@ -2254,10 +2248,10 @@
         <v>63</v>
       </c>
       <c r="B57" s="0" t="n">
-        <v>2863.113</v>
+        <v>2899.866</v>
       </c>
       <c r="C57" s="0" t="n">
-        <v>157.619</v>
+        <v>157.782</v>
       </c>
       <c r="D57" s="0" t="n">
         <v>41.965</v>
@@ -2266,7 +2260,7 @@
         <v>2.256</v>
       </c>
       <c r="F57" s="0" t="n">
-        <v>2.942</v>
+        <v>3.311</v>
       </c>
       <c r="G57" s="0" t="n">
         <v>1.188</v>
@@ -2280,10 +2274,10 @@
         <v>64</v>
       </c>
       <c r="B58" s="0" t="n">
-        <v>2863.331</v>
+        <v>2899.866</v>
       </c>
       <c r="C58" s="0" t="n">
-        <v>157.619</v>
+        <v>157.782</v>
       </c>
       <c r="D58" s="0" t="n">
         <v>41.965</v>
@@ -2292,7 +2286,7 @@
         <v>2.256</v>
       </c>
       <c r="F58" s="0" t="n">
-        <v>2.942</v>
+        <v>3.563</v>
       </c>
       <c r="G58" s="0" t="n">
         <v>1.188</v>
@@ -2306,19 +2300,19 @@
         <v>65</v>
       </c>
       <c r="B59" s="0" t="n">
-        <v>2863.721</v>
+        <v>2899.866</v>
       </c>
       <c r="C59" s="0" t="n">
-        <v>157.619</v>
+        <v>157.782</v>
       </c>
       <c r="D59" s="0" t="n">
-        <v>41.965</v>
+        <v>42.191</v>
       </c>
       <c r="E59" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F59" s="0" t="n">
-        <v>2.942</v>
+        <v>3.563</v>
       </c>
       <c r="G59" s="0" t="n">
         <v>1.188</v>
@@ -2332,19 +2326,19 @@
         <v>66</v>
       </c>
       <c r="B60" s="0" t="n">
-        <v>2863.721</v>
+        <v>2899.866</v>
       </c>
       <c r="C60" s="0" t="n">
-        <v>157.619</v>
+        <v>157.782</v>
       </c>
       <c r="D60" s="0" t="n">
-        <v>41.965</v>
+        <v>42.191</v>
       </c>
       <c r="E60" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F60" s="0" t="n">
-        <v>2.942</v>
+        <v>3.563</v>
       </c>
       <c r="G60" s="0" t="n">
         <v>1.188</v>
@@ -2358,19 +2352,19 @@
         <v>67</v>
       </c>
       <c r="B61" s="0" t="n">
-        <v>2864.183</v>
+        <v>2900.388</v>
       </c>
       <c r="C61" s="0" t="n">
-        <v>157.619</v>
+        <v>157.782</v>
       </c>
       <c r="D61" s="0" t="n">
-        <v>41.965</v>
+        <v>42.191</v>
       </c>
       <c r="E61" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F61" s="0" t="n">
-        <v>2.942</v>
+        <v>3.563</v>
       </c>
       <c r="G61" s="0" t="n">
         <v>1.188</v>
@@ -2384,19 +2378,19 @@
         <v>68</v>
       </c>
       <c r="B62" s="0" t="n">
-        <v>2864.183</v>
+        <v>2900.388</v>
       </c>
       <c r="C62" s="0" t="n">
-        <v>157.619</v>
+        <v>157.782</v>
       </c>
       <c r="D62" s="0" t="n">
-        <v>41.965</v>
+        <v>42.191</v>
       </c>
       <c r="E62" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F62" s="0" t="n">
-        <v>2.942</v>
+        <v>3.563</v>
       </c>
       <c r="G62" s="0" t="n">
         <v>1.188</v>
@@ -2410,19 +2404,19 @@
         <v>69</v>
       </c>
       <c r="B63" s="0" t="n">
-        <v>2864.404</v>
+        <v>2900.388</v>
       </c>
       <c r="C63" s="0" t="n">
-        <v>157.619</v>
+        <v>157.782</v>
       </c>
       <c r="D63" s="0" t="n">
-        <v>41.965</v>
+        <v>42.191</v>
       </c>
       <c r="E63" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F63" s="0" t="n">
-        <v>2.942</v>
+        <v>3.793</v>
       </c>
       <c r="G63" s="0" t="n">
         <v>1.188</v>
@@ -2436,19 +2430,19 @@
         <v>70</v>
       </c>
       <c r="B64" s="0" t="n">
-        <v>2864.404</v>
+        <v>2900.388</v>
       </c>
       <c r="C64" s="0" t="n">
-        <v>157.619</v>
+        <v>157.782</v>
       </c>
       <c r="D64" s="0" t="n">
-        <v>41.965</v>
+        <v>42.416</v>
       </c>
       <c r="E64" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F64" s="0" t="n">
-        <v>2.942</v>
+        <v>3.793</v>
       </c>
       <c r="G64" s="0" t="n">
         <v>1.188</v>
@@ -2462,19 +2456,19 @@
         <v>71</v>
       </c>
       <c r="B65" s="0" t="n">
-        <v>2875.844</v>
+        <v>2900.388</v>
       </c>
       <c r="C65" s="0" t="n">
-        <v>157.619</v>
+        <v>157.835</v>
       </c>
       <c r="D65" s="0" t="n">
-        <v>41.965</v>
+        <v>42.65</v>
       </c>
       <c r="E65" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F65" s="0" t="n">
-        <v>2.942</v>
+        <v>3.793</v>
       </c>
       <c r="G65" s="0" t="n">
         <v>1.188</v>
@@ -2488,19 +2482,19 @@
         <v>72</v>
       </c>
       <c r="B66" s="0" t="n">
-        <v>2875.844</v>
+        <v>2912.717</v>
       </c>
       <c r="C66" s="0" t="n">
-        <v>157.619</v>
+        <v>159.561</v>
       </c>
       <c r="D66" s="0" t="n">
-        <v>41.965</v>
+        <v>42.65</v>
       </c>
       <c r="E66" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F66" s="0" t="n">
-        <v>2.942</v>
+        <v>3.793</v>
       </c>
       <c r="G66" s="0" t="n">
         <v>1.188</v>
@@ -2514,19 +2508,19 @@
         <v>73</v>
       </c>
       <c r="B67" s="0" t="n">
-        <v>2875.844</v>
+        <v>2924.242</v>
       </c>
       <c r="C67" s="0" t="n">
-        <v>157.619</v>
+        <v>159.561</v>
       </c>
       <c r="D67" s="0" t="n">
-        <v>41.965</v>
+        <v>42.65</v>
       </c>
       <c r="E67" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F67" s="0" t="n">
-        <v>2.942</v>
+        <v>3.793</v>
       </c>
       <c r="G67" s="0" t="n">
         <v>1.188</v>
@@ -2540,19 +2534,19 @@
         <v>74</v>
       </c>
       <c r="B68" s="0" t="n">
-        <v>2875.844</v>
+        <v>2924.242</v>
       </c>
       <c r="C68" s="0" t="n">
-        <v>157.619</v>
+        <v>159.561</v>
       </c>
       <c r="D68" s="0" t="n">
-        <v>41.965</v>
+        <v>42.65</v>
       </c>
       <c r="E68" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F68" s="0" t="n">
-        <v>2.942</v>
+        <v>3.793</v>
       </c>
       <c r="G68" s="0" t="n">
         <v>1.188</v>
@@ -2566,19 +2560,19 @@
         <v>75</v>
       </c>
       <c r="B69" s="0" t="n">
-        <v>2875.853</v>
+        <v>2924.242</v>
       </c>
       <c r="C69" s="0" t="n">
-        <v>157.619</v>
+        <v>159.561</v>
       </c>
       <c r="D69" s="0" t="n">
-        <v>41.965</v>
+        <v>42.65</v>
       </c>
       <c r="E69" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F69" s="0" t="n">
-        <v>2.942</v>
+        <v>3.793</v>
       </c>
       <c r="G69" s="0" t="n">
         <v>1.188</v>
@@ -2592,19 +2586,19 @@
         <v>76</v>
       </c>
       <c r="B70" s="0" t="n">
-        <v>2876.161</v>
+        <v>2924.242</v>
       </c>
       <c r="C70" s="0" t="n">
-        <v>157.619</v>
+        <v>159.561</v>
       </c>
       <c r="D70" s="0" t="n">
-        <v>41.965</v>
+        <v>42.65</v>
       </c>
       <c r="E70" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F70" s="0" t="n">
-        <v>2.942</v>
+        <v>3.793</v>
       </c>
       <c r="G70" s="0" t="n">
         <v>1.188</v>
@@ -2618,19 +2612,19 @@
         <v>77</v>
       </c>
       <c r="B71" s="0" t="n">
-        <v>2876.161</v>
+        <v>2924.242</v>
       </c>
       <c r="C71" s="0" t="n">
-        <v>157.619</v>
+        <v>159.561</v>
       </c>
       <c r="D71" s="0" t="n">
-        <v>41.965</v>
+        <v>42.665</v>
       </c>
       <c r="E71" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F71" s="0" t="n">
-        <v>2.942</v>
+        <v>3.793</v>
       </c>
       <c r="G71" s="0" t="n">
         <v>1.188</v>
@@ -2644,19 +2638,19 @@
         <v>78</v>
       </c>
       <c r="B72" s="0" t="n">
-        <v>2876.397</v>
+        <v>2924.242</v>
       </c>
       <c r="C72" s="0" t="n">
-        <v>157.619</v>
+        <v>159.561</v>
       </c>
       <c r="D72" s="0" t="n">
-        <v>41.965</v>
+        <v>42.665</v>
       </c>
       <c r="E72" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F72" s="0" t="n">
-        <v>2.942</v>
+        <v>3.793</v>
       </c>
       <c r="G72" s="0" t="n">
         <v>1.188</v>
@@ -2670,19 +2664,19 @@
         <v>79</v>
       </c>
       <c r="B73" s="0" t="n">
-        <v>2886.936</v>
+        <v>2931.72</v>
       </c>
       <c r="C73" s="0" t="n">
-        <v>157.782</v>
+        <v>159.561</v>
       </c>
       <c r="D73" s="0" t="n">
-        <v>41.965</v>
+        <v>43.124</v>
       </c>
       <c r="E73" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F73" s="0" t="n">
-        <v>2.942</v>
+        <v>3.793</v>
       </c>
       <c r="G73" s="0" t="n">
         <v>1.188</v>
@@ -2696,19 +2690,19 @@
         <v>80</v>
       </c>
       <c r="B74" s="0" t="n">
-        <v>2887.492</v>
+        <v>2950.048</v>
       </c>
       <c r="C74" s="0" t="n">
-        <v>157.782</v>
+        <v>159.561</v>
       </c>
       <c r="D74" s="0" t="n">
-        <v>41.965</v>
+        <v>43.124</v>
       </c>
       <c r="E74" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F74" s="0" t="n">
-        <v>2.942</v>
+        <v>3.793</v>
       </c>
       <c r="G74" s="0" t="n">
         <v>1.188</v>
@@ -2722,19 +2716,19 @@
         <v>81</v>
       </c>
       <c r="B75" s="0" t="n">
-        <v>2887.771</v>
+        <v>2950.048</v>
       </c>
       <c r="C75" s="0" t="n">
-        <v>157.782</v>
+        <v>159.561</v>
       </c>
       <c r="D75" s="0" t="n">
-        <v>41.965</v>
+        <v>43.729</v>
       </c>
       <c r="E75" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F75" s="0" t="n">
-        <v>2.942</v>
+        <v>3.793</v>
       </c>
       <c r="G75" s="0" t="n">
         <v>1.188</v>
@@ -2748,19 +2742,19 @@
         <v>82</v>
       </c>
       <c r="B76" s="0" t="n">
-        <v>2887.771</v>
+        <v>2950.048</v>
       </c>
       <c r="C76" s="0" t="n">
-        <v>157.782</v>
+        <v>159.561</v>
       </c>
       <c r="D76" s="0" t="n">
-        <v>41.965</v>
+        <v>43.729</v>
       </c>
       <c r="E76" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F76" s="0" t="n">
-        <v>2.942</v>
+        <v>3.793</v>
       </c>
       <c r="G76" s="0" t="n">
         <v>1.188</v>
@@ -2774,19 +2768,19 @@
         <v>83</v>
       </c>
       <c r="B77" s="0" t="n">
-        <v>2887.771</v>
+        <v>2950.356</v>
       </c>
       <c r="C77" s="0" t="n">
-        <v>157.782</v>
+        <v>159.561</v>
       </c>
       <c r="D77" s="0" t="n">
-        <v>41.965</v>
+        <v>43.729</v>
       </c>
       <c r="E77" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F77" s="0" t="n">
-        <v>2.942</v>
+        <v>3.793</v>
       </c>
       <c r="G77" s="0" t="n">
         <v>1.188</v>
@@ -2800,19 +2794,19 @@
         <v>84</v>
       </c>
       <c r="B78" s="0" t="n">
-        <v>2888</v>
+        <v>2950.356</v>
       </c>
       <c r="C78" s="0" t="n">
-        <v>157.782</v>
+        <v>159.561</v>
       </c>
       <c r="D78" s="0" t="n">
-        <v>41.965</v>
+        <v>43.729</v>
       </c>
       <c r="E78" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F78" s="0" t="n">
-        <v>2.942</v>
+        <v>3.793</v>
       </c>
       <c r="G78" s="0" t="n">
         <v>1.188</v>
@@ -2826,19 +2820,19 @@
         <v>85</v>
       </c>
       <c r="B79" s="0" t="n">
-        <v>2888</v>
+        <v>2963.804</v>
       </c>
       <c r="C79" s="0" t="n">
-        <v>157.782</v>
+        <v>164.049</v>
       </c>
       <c r="D79" s="0" t="n">
-        <v>41.965</v>
+        <v>43.729</v>
       </c>
       <c r="E79" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F79" s="0" t="n">
-        <v>2.942</v>
+        <v>3.793</v>
       </c>
       <c r="G79" s="0" t="n">
         <v>1.188</v>
@@ -2852,19 +2846,19 @@
         <v>86</v>
       </c>
       <c r="B80" s="0" t="n">
-        <v>2899.866</v>
+        <v>2963.804</v>
       </c>
       <c r="C80" s="0" t="n">
-        <v>157.782</v>
+        <v>164.049</v>
       </c>
       <c r="D80" s="0" t="n">
-        <v>41.965</v>
+        <v>43.729</v>
       </c>
       <c r="E80" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F80" s="0" t="n">
-        <v>2.942</v>
+        <v>3.793</v>
       </c>
       <c r="G80" s="0" t="n">
         <v>1.188</v>
@@ -2878,19 +2872,19 @@
         <v>87</v>
       </c>
       <c r="B81" s="0" t="n">
-        <v>2899.866</v>
+        <v>2963.804</v>
       </c>
       <c r="C81" s="0" t="n">
-        <v>157.782</v>
+        <v>164.049</v>
       </c>
       <c r="D81" s="0" t="n">
-        <v>41.965</v>
+        <v>43.729</v>
       </c>
       <c r="E81" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F81" s="0" t="n">
-        <v>2.942</v>
+        <v>3.793</v>
       </c>
       <c r="G81" s="0" t="n">
         <v>1.188</v>
@@ -2904,19 +2898,19 @@
         <v>88</v>
       </c>
       <c r="B82" s="0" t="n">
-        <v>2899.866</v>
+        <v>2971.367</v>
       </c>
       <c r="C82" s="0" t="n">
-        <v>157.782</v>
+        <v>164.049</v>
       </c>
       <c r="D82" s="0" t="n">
-        <v>41.965</v>
+        <v>43.729</v>
       </c>
       <c r="E82" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F82" s="0" t="n">
-        <v>2.942</v>
+        <v>3.793</v>
       </c>
       <c r="G82" s="0" t="n">
         <v>1.188</v>
@@ -2930,19 +2924,19 @@
         <v>89</v>
       </c>
       <c r="B83" s="0" t="n">
-        <v>2899.866</v>
+        <v>2980.453</v>
       </c>
       <c r="C83" s="0" t="n">
-        <v>157.782</v>
+        <v>164.049</v>
       </c>
       <c r="D83" s="0" t="n">
-        <v>41.965</v>
+        <v>43.729</v>
       </c>
       <c r="E83" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F83" s="0" t="n">
-        <v>2.942</v>
+        <v>3.793</v>
       </c>
       <c r="G83" s="0" t="n">
         <v>1.188</v>
@@ -2956,19 +2950,19 @@
         <v>90</v>
       </c>
       <c r="B84" s="0" t="n">
-        <v>2899.866</v>
+        <v>2997.787</v>
       </c>
       <c r="C84" s="0" t="n">
-        <v>157.782</v>
+        <v>164.049</v>
       </c>
       <c r="D84" s="0" t="n">
-        <v>41.965</v>
+        <v>43.729</v>
       </c>
       <c r="E84" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F84" s="0" t="n">
-        <v>3.311</v>
+        <v>3.793</v>
       </c>
       <c r="G84" s="0" t="n">
         <v>1.188</v>
@@ -2982,19 +2976,19 @@
         <v>91</v>
       </c>
       <c r="B85" s="0" t="n">
-        <v>2899.866</v>
+        <v>2997.787</v>
       </c>
       <c r="C85" s="0" t="n">
-        <v>157.782</v>
+        <v>164.049</v>
       </c>
       <c r="D85" s="0" t="n">
-        <v>41.965</v>
+        <v>43.729</v>
       </c>
       <c r="E85" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F85" s="0" t="n">
-        <v>3.311</v>
+        <v>3.793</v>
       </c>
       <c r="G85" s="0" t="n">
         <v>1.188</v>
@@ -3008,19 +3002,19 @@
         <v>92</v>
       </c>
       <c r="B86" s="0" t="n">
-        <v>2899.866</v>
+        <v>2997.787</v>
       </c>
       <c r="C86" s="0" t="n">
-        <v>157.782</v>
+        <v>164.049</v>
       </c>
       <c r="D86" s="0" t="n">
-        <v>41.965</v>
+        <v>43.729</v>
       </c>
       <c r="E86" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F86" s="0" t="n">
-        <v>3.563</v>
+        <v>3.793</v>
       </c>
       <c r="G86" s="0" t="n">
         <v>1.188</v>
@@ -3034,19 +3028,19 @@
         <v>93</v>
       </c>
       <c r="B87" s="0" t="n">
-        <v>2899.866</v>
+        <v>2997.787</v>
       </c>
       <c r="C87" s="0" t="n">
-        <v>157.782</v>
+        <v>164.049</v>
       </c>
       <c r="D87" s="0" t="n">
-        <v>42.191</v>
+        <v>43.729</v>
       </c>
       <c r="E87" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F87" s="0" t="n">
-        <v>3.563</v>
+        <v>3.793</v>
       </c>
       <c r="G87" s="0" t="n">
         <v>1.188</v>
@@ -3060,19 +3054,19 @@
         <v>94</v>
       </c>
       <c r="B88" s="0" t="n">
-        <v>2899.866</v>
+        <v>2997.787</v>
       </c>
       <c r="C88" s="0" t="n">
-        <v>157.782</v>
+        <v>164.049</v>
       </c>
       <c r="D88" s="0" t="n">
-        <v>42.191</v>
+        <v>43.729</v>
       </c>
       <c r="E88" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F88" s="0" t="n">
-        <v>3.563</v>
+        <v>3.793</v>
       </c>
       <c r="G88" s="0" t="n">
         <v>1.188</v>
@@ -3086,19 +3080,19 @@
         <v>95</v>
       </c>
       <c r="B89" s="0" t="n">
-        <v>2900.388</v>
+        <v>2997.787</v>
       </c>
       <c r="C89" s="0" t="n">
-        <v>157.782</v>
+        <v>164.049</v>
       </c>
       <c r="D89" s="0" t="n">
-        <v>42.191</v>
+        <v>43.729</v>
       </c>
       <c r="E89" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F89" s="0" t="n">
-        <v>3.563</v>
+        <v>3.793</v>
       </c>
       <c r="G89" s="0" t="n">
         <v>1.188</v>
@@ -3112,19 +3106,19 @@
         <v>96</v>
       </c>
       <c r="B90" s="0" t="n">
-        <v>2900.388</v>
+        <v>2997.787</v>
       </c>
       <c r="C90" s="0" t="n">
-        <v>157.782</v>
+        <v>164.049</v>
       </c>
       <c r="D90" s="0" t="n">
-        <v>42.191</v>
+        <v>43.729</v>
       </c>
       <c r="E90" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F90" s="0" t="n">
-        <v>3.563</v>
+        <v>3.793</v>
       </c>
       <c r="G90" s="0" t="n">
         <v>1.188</v>
@@ -3138,13 +3132,13 @@
         <v>97</v>
       </c>
       <c r="B91" s="0" t="n">
-        <v>2900.388</v>
+        <v>2997.787</v>
       </c>
       <c r="C91" s="0" t="n">
-        <v>157.782</v>
+        <v>164.049</v>
       </c>
       <c r="D91" s="0" t="n">
-        <v>42.191</v>
+        <v>43.729</v>
       </c>
       <c r="E91" s="0" t="n">
         <v>2.256</v>
@@ -3164,13 +3158,13 @@
         <v>98</v>
       </c>
       <c r="B92" s="0" t="n">
-        <v>2900.388</v>
+        <v>2997.787</v>
       </c>
       <c r="C92" s="0" t="n">
-        <v>157.782</v>
+        <v>164.049</v>
       </c>
       <c r="D92" s="0" t="n">
-        <v>42.416</v>
+        <v>43.729</v>
       </c>
       <c r="E92" s="0" t="n">
         <v>2.256</v>
@@ -3190,13 +3184,13 @@
         <v>99</v>
       </c>
       <c r="B93" s="0" t="n">
-        <v>2900.388</v>
+        <v>2997.787</v>
       </c>
       <c r="C93" s="0" t="n">
-        <v>157.835</v>
+        <v>164.049</v>
       </c>
       <c r="D93" s="0" t="n">
-        <v>42.65</v>
+        <v>43.736</v>
       </c>
       <c r="E93" s="0" t="n">
         <v>2.256</v>
@@ -3216,13 +3210,13 @@
         <v>100</v>
       </c>
       <c r="B94" s="0" t="n">
-        <v>2912.717</v>
+        <v>2997.937</v>
       </c>
       <c r="C94" s="0" t="n">
-        <v>159.561</v>
+        <v>164.049</v>
       </c>
       <c r="D94" s="0" t="n">
-        <v>42.65</v>
+        <v>43.736</v>
       </c>
       <c r="E94" s="0" t="n">
         <v>2.256</v>
@@ -3242,13 +3236,13 @@
         <v>101</v>
       </c>
       <c r="B95" s="0" t="n">
-        <v>2924.242</v>
+        <v>2997.937</v>
       </c>
       <c r="C95" s="0" t="n">
-        <v>159.561</v>
+        <v>164.049</v>
       </c>
       <c r="D95" s="0" t="n">
-        <v>42.65</v>
+        <v>43.736</v>
       </c>
       <c r="E95" s="0" t="n">
         <v>2.256</v>
@@ -3268,19 +3262,19 @@
         <v>102</v>
       </c>
       <c r="B96" s="0" t="n">
-        <v>2924.242</v>
+        <v>2997.937</v>
       </c>
       <c r="C96" s="0" t="n">
-        <v>159.561</v>
+        <v>164.049</v>
       </c>
       <c r="D96" s="0" t="n">
-        <v>42.65</v>
+        <v>43.736</v>
       </c>
       <c r="E96" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F96" s="0" t="n">
-        <v>3.793</v>
+        <v>4.549</v>
       </c>
       <c r="G96" s="0" t="n">
         <v>1.188</v>
@@ -3294,19 +3288,19 @@
         <v>103</v>
       </c>
       <c r="B97" s="0" t="n">
-        <v>2924.242</v>
+        <v>2997.937</v>
       </c>
       <c r="C97" s="0" t="n">
-        <v>159.561</v>
+        <v>164.049</v>
       </c>
       <c r="D97" s="0" t="n">
-        <v>42.65</v>
+        <v>43.736</v>
       </c>
       <c r="E97" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F97" s="0" t="n">
-        <v>3.793</v>
+        <v>4.949</v>
       </c>
       <c r="G97" s="0" t="n">
         <v>1.188</v>
@@ -3320,19 +3314,19 @@
         <v>104</v>
       </c>
       <c r="B98" s="0" t="n">
-        <v>2924.242</v>
+        <v>2997.937</v>
       </c>
       <c r="C98" s="0" t="n">
-        <v>159.561</v>
+        <v>164.049</v>
       </c>
       <c r="D98" s="0" t="n">
-        <v>42.65</v>
+        <v>43.736</v>
       </c>
       <c r="E98" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F98" s="0" t="n">
-        <v>3.793</v>
+        <v>4.949</v>
       </c>
       <c r="G98" s="0" t="n">
         <v>1.188</v>
@@ -3346,19 +3340,19 @@
         <v>105</v>
       </c>
       <c r="B99" s="0" t="n">
-        <v>2924.242</v>
+        <v>2997.937</v>
       </c>
       <c r="C99" s="0" t="n">
-        <v>159.561</v>
+        <v>164.049</v>
       </c>
       <c r="D99" s="0" t="n">
-        <v>42.665</v>
+        <v>43.736</v>
       </c>
       <c r="E99" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F99" s="0" t="n">
-        <v>3.793</v>
+        <v>4.949</v>
       </c>
       <c r="G99" s="0" t="n">
         <v>1.188</v>
@@ -3372,19 +3366,19 @@
         <v>106</v>
       </c>
       <c r="B100" s="0" t="n">
-        <v>2924.242</v>
+        <v>2997.937</v>
       </c>
       <c r="C100" s="0" t="n">
-        <v>159.561</v>
+        <v>164.049</v>
       </c>
       <c r="D100" s="0" t="n">
-        <v>42.665</v>
+        <v>43.736</v>
       </c>
       <c r="E100" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F100" s="0" t="n">
-        <v>3.793</v>
+        <v>4.949</v>
       </c>
       <c r="G100" s="0" t="n">
         <v>1.188</v>
@@ -3398,19 +3392,19 @@
         <v>107</v>
       </c>
       <c r="B101" s="0" t="n">
-        <v>2931.72</v>
+        <v>3005.43</v>
       </c>
       <c r="C101" s="0" t="n">
-        <v>159.561</v>
+        <v>164.049</v>
       </c>
       <c r="D101" s="0" t="n">
-        <v>43.124</v>
+        <v>43.736</v>
       </c>
       <c r="E101" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F101" s="0" t="n">
-        <v>3.793</v>
+        <v>4.949</v>
       </c>
       <c r="G101" s="0" t="n">
         <v>1.188</v>
@@ -3424,19 +3418,19 @@
         <v>108</v>
       </c>
       <c r="B102" s="0" t="n">
-        <v>2950.048</v>
+        <v>3010.782</v>
       </c>
       <c r="C102" s="0" t="n">
-        <v>159.561</v>
+        <v>164.049</v>
       </c>
       <c r="D102" s="0" t="n">
-        <v>43.124</v>
+        <v>43.736</v>
       </c>
       <c r="E102" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F102" s="0" t="n">
-        <v>3.793</v>
+        <v>4.949</v>
       </c>
       <c r="G102" s="0" t="n">
         <v>1.188</v>
@@ -3450,19 +3444,19 @@
         <v>109</v>
       </c>
       <c r="B103" s="0" t="n">
-        <v>2950.048</v>
+        <v>3010.782</v>
       </c>
       <c r="C103" s="0" t="n">
-        <v>159.561</v>
+        <v>164.049</v>
       </c>
       <c r="D103" s="0" t="n">
-        <v>43.729</v>
+        <v>43.736</v>
       </c>
       <c r="E103" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F103" s="0" t="n">
-        <v>3.793</v>
+        <v>4.949</v>
       </c>
       <c r="G103" s="0" t="n">
         <v>1.188</v>
@@ -3476,19 +3470,19 @@
         <v>110</v>
       </c>
       <c r="B104" s="0" t="n">
-        <v>2950.048</v>
+        <v>3010.782</v>
       </c>
       <c r="C104" s="0" t="n">
-        <v>159.561</v>
+        <v>164.049</v>
       </c>
       <c r="D104" s="0" t="n">
-        <v>43.729</v>
+        <v>43.971</v>
       </c>
       <c r="E104" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F104" s="0" t="n">
-        <v>3.793</v>
+        <v>4.949</v>
       </c>
       <c r="G104" s="0" t="n">
         <v>1.188</v>
@@ -3502,19 +3496,19 @@
         <v>111</v>
       </c>
       <c r="B105" s="0" t="n">
-        <v>2950.356</v>
+        <v>3010.782</v>
       </c>
       <c r="C105" s="0" t="n">
-        <v>159.561</v>
+        <v>164.049</v>
       </c>
       <c r="D105" s="0" t="n">
-        <v>43.729</v>
+        <v>43.971</v>
       </c>
       <c r="E105" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F105" s="0" t="n">
-        <v>3.793</v>
+        <v>5.216</v>
       </c>
       <c r="G105" s="0" t="n">
         <v>1.188</v>
@@ -3528,19 +3522,19 @@
         <v>112</v>
       </c>
       <c r="B106" s="0" t="n">
-        <v>2950.356</v>
+        <v>3010.782</v>
       </c>
       <c r="C106" s="0" t="n">
-        <v>159.561</v>
+        <v>164.049</v>
       </c>
       <c r="D106" s="0" t="n">
-        <v>43.729</v>
+        <v>43.971</v>
       </c>
       <c r="E106" s="0" t="n">
         <v>2.256</v>
       </c>
       <c r="F106" s="0" t="n">
-        <v>3.793</v>
+        <v>5.442</v>
       </c>
       <c r="G106" s="0" t="n">
         <v>1.188</v>
@@ -3554,19 +3548,19 @@
         <v>113</v>
       </c>
       <c r="B107" s="0" t="n">
-        <v>2963.804</v>
+        <v>3010.782</v>
       </c>
       <c r="C107" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D107" s="0" t="n">
-        <v>43.729</v>
+        <v>43.971</v>
       </c>
       <c r="E107" s="0" t="n">
-        <v>2.256</v>
+        <v>2.362</v>
       </c>
       <c r="F107" s="0" t="n">
-        <v>3.793</v>
+        <v>5.442</v>
       </c>
       <c r="G107" s="0" t="n">
         <v>1.188</v>
@@ -3580,19 +3574,19 @@
         <v>114</v>
       </c>
       <c r="B108" s="0" t="n">
-        <v>2963.804</v>
+        <v>3018.213</v>
       </c>
       <c r="C108" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D108" s="0" t="n">
-        <v>43.729</v>
+        <v>43.971</v>
       </c>
       <c r="E108" s="0" t="n">
-        <v>2.256</v>
+        <v>2.362</v>
       </c>
       <c r="F108" s="0" t="n">
-        <v>3.793</v>
+        <v>5.442</v>
       </c>
       <c r="G108" s="0" t="n">
         <v>1.188</v>
@@ -3606,19 +3600,19 @@
         <v>115</v>
       </c>
       <c r="B109" s="0" t="n">
-        <v>2963.804</v>
+        <v>3027.483</v>
       </c>
       <c r="C109" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D109" s="0" t="n">
-        <v>43.729</v>
+        <v>43.971</v>
       </c>
       <c r="E109" s="0" t="n">
-        <v>2.256</v>
+        <v>2.362</v>
       </c>
       <c r="F109" s="0" t="n">
-        <v>3.793</v>
+        <v>5.442</v>
       </c>
       <c r="G109" s="0" t="n">
         <v>1.188</v>
@@ -3632,19 +3626,19 @@
         <v>116</v>
       </c>
       <c r="B110" s="0" t="n">
-        <v>2971.367</v>
+        <v>3037.77</v>
       </c>
       <c r="C110" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D110" s="0" t="n">
-        <v>43.729</v>
+        <v>43.971</v>
       </c>
       <c r="E110" s="0" t="n">
-        <v>2.256</v>
+        <v>2.362</v>
       </c>
       <c r="F110" s="0" t="n">
-        <v>3.793</v>
+        <v>5.442</v>
       </c>
       <c r="G110" s="0" t="n">
         <v>1.188</v>
@@ -3658,19 +3652,19 @@
         <v>117</v>
       </c>
       <c r="B111" s="0" t="n">
-        <v>2980.453</v>
+        <v>3037.77</v>
       </c>
       <c r="C111" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D111" s="0" t="n">
-        <v>43.729</v>
+        <v>43.971</v>
       </c>
       <c r="E111" s="0" t="n">
-        <v>2.256</v>
+        <v>2.362</v>
       </c>
       <c r="F111" s="0" t="n">
-        <v>3.793</v>
+        <v>5.442</v>
       </c>
       <c r="G111" s="0" t="n">
         <v>1.188</v>
@@ -3684,19 +3678,19 @@
         <v>118</v>
       </c>
       <c r="B112" s="0" t="n">
-        <v>2997.787</v>
+        <v>3037.77</v>
       </c>
       <c r="C112" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D112" s="0" t="n">
-        <v>43.729</v>
+        <v>43.971</v>
       </c>
       <c r="E112" s="0" t="n">
-        <v>2.256</v>
+        <v>2.362</v>
       </c>
       <c r="F112" s="0" t="n">
-        <v>3.793</v>
+        <v>5.442</v>
       </c>
       <c r="G112" s="0" t="n">
         <v>1.188</v>
@@ -3710,19 +3704,19 @@
         <v>119</v>
       </c>
       <c r="B113" s="0" t="n">
-        <v>2997.787</v>
+        <v>3037.77</v>
       </c>
       <c r="C113" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D113" s="0" t="n">
-        <v>43.729</v>
+        <v>43.979</v>
       </c>
       <c r="E113" s="0" t="n">
-        <v>2.256</v>
+        <v>2.362</v>
       </c>
       <c r="F113" s="0" t="n">
-        <v>3.793</v>
+        <v>5.442</v>
       </c>
       <c r="G113" s="0" t="n">
         <v>1.188</v>
@@ -3736,19 +3730,19 @@
         <v>120</v>
       </c>
       <c r="B114" s="0" t="n">
-        <v>2997.787</v>
+        <v>3045.333</v>
       </c>
       <c r="C114" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D114" s="0" t="n">
-        <v>43.729</v>
+        <v>43.979</v>
       </c>
       <c r="E114" s="0" t="n">
-        <v>2.256</v>
+        <v>2.362</v>
       </c>
       <c r="F114" s="0" t="n">
-        <v>3.793</v>
+        <v>5.442</v>
       </c>
       <c r="G114" s="0" t="n">
         <v>1.188</v>
@@ -3762,19 +3756,19 @@
         <v>121</v>
       </c>
       <c r="B115" s="0" t="n">
-        <v>2997.787</v>
+        <v>3067.38</v>
       </c>
       <c r="C115" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D115" s="0" t="n">
-        <v>43.729</v>
+        <v>43.979</v>
       </c>
       <c r="E115" s="0" t="n">
-        <v>2.256</v>
+        <v>2.362</v>
       </c>
       <c r="F115" s="0" t="n">
-        <v>3.793</v>
+        <v>5.442</v>
       </c>
       <c r="G115" s="0" t="n">
         <v>1.188</v>
@@ -3788,19 +3782,19 @@
         <v>122</v>
       </c>
       <c r="B116" s="0" t="n">
-        <v>2997.787</v>
+        <v>3067.38</v>
       </c>
       <c r="C116" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D116" s="0" t="n">
-        <v>43.729</v>
+        <v>44.017</v>
       </c>
       <c r="E116" s="0" t="n">
-        <v>2.256</v>
+        <v>2.416</v>
       </c>
       <c r="F116" s="0" t="n">
-        <v>3.793</v>
+        <v>5.442</v>
       </c>
       <c r="G116" s="0" t="n">
         <v>1.188</v>
@@ -3814,25 +3808,25 @@
         <v>123</v>
       </c>
       <c r="B117" s="0" t="n">
-        <v>2997.787</v>
+        <v>3067.38</v>
       </c>
       <c r="C117" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D117" s="0" t="n">
-        <v>43.729</v>
+        <v>44.069</v>
       </c>
       <c r="E117" s="0" t="n">
-        <v>2.256</v>
+        <v>2.416</v>
       </c>
       <c r="F117" s="0" t="n">
-        <v>3.793</v>
+        <v>5.442</v>
       </c>
       <c r="G117" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H117" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3840,25 +3834,25 @@
         <v>124</v>
       </c>
       <c r="B118" s="0" t="n">
-        <v>2997.787</v>
+        <v>3067.38</v>
       </c>
       <c r="C118" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D118" s="0" t="n">
-        <v>43.729</v>
+        <v>44.069</v>
       </c>
       <c r="E118" s="0" t="n">
-        <v>2.256</v>
+        <v>2.416</v>
       </c>
       <c r="F118" s="0" t="n">
-        <v>3.793</v>
+        <v>5.442</v>
       </c>
       <c r="G118" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H118" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3866,25 +3860,25 @@
         <v>125</v>
       </c>
       <c r="B119" s="0" t="n">
-        <v>2997.787</v>
+        <v>3067.856</v>
       </c>
       <c r="C119" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D119" s="0" t="n">
-        <v>43.729</v>
+        <v>44.069</v>
       </c>
       <c r="E119" s="0" t="n">
-        <v>2.256</v>
+        <v>2.416</v>
       </c>
       <c r="F119" s="0" t="n">
-        <v>3.793</v>
+        <v>5.442</v>
       </c>
       <c r="G119" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H119" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3892,25 +3886,25 @@
         <v>126</v>
       </c>
       <c r="B120" s="0" t="n">
-        <v>2997.787</v>
+        <v>3068.084</v>
       </c>
       <c r="C120" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D120" s="0" t="n">
-        <v>43.729</v>
+        <v>44.069</v>
       </c>
       <c r="E120" s="0" t="n">
-        <v>2.256</v>
+        <v>2.416</v>
       </c>
       <c r="F120" s="0" t="n">
-        <v>3.793</v>
+        <v>5.442</v>
       </c>
       <c r="G120" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H120" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3918,25 +3912,25 @@
         <v>127</v>
       </c>
       <c r="B121" s="0" t="n">
-        <v>2997.787</v>
+        <v>3068.314</v>
       </c>
       <c r="C121" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D121" s="0" t="n">
-        <v>43.736</v>
+        <v>44.069</v>
       </c>
       <c r="E121" s="0" t="n">
-        <v>2.256</v>
+        <v>2.416</v>
       </c>
       <c r="F121" s="0" t="n">
-        <v>3.793</v>
+        <v>5.442</v>
       </c>
       <c r="G121" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H121" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3944,25 +3938,25 @@
         <v>128</v>
       </c>
       <c r="B122" s="0" t="n">
-        <v>2997.937</v>
+        <v>3068.314</v>
       </c>
       <c r="C122" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D122" s="0" t="n">
-        <v>43.736</v>
+        <v>44.069</v>
       </c>
       <c r="E122" s="0" t="n">
-        <v>2.256</v>
+        <v>2.416</v>
       </c>
       <c r="F122" s="0" t="n">
-        <v>3.793</v>
+        <v>5.442</v>
       </c>
       <c r="G122" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H122" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3970,25 +3964,25 @@
         <v>129</v>
       </c>
       <c r="B123" s="0" t="n">
-        <v>2997.937</v>
+        <v>3068.314</v>
       </c>
       <c r="C123" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D123" s="0" t="n">
-        <v>43.736</v>
+        <v>44.069</v>
       </c>
       <c r="E123" s="0" t="n">
-        <v>2.256</v>
+        <v>2.416</v>
       </c>
       <c r="F123" s="0" t="n">
-        <v>3.793</v>
+        <v>5.69</v>
       </c>
       <c r="G123" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H123" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3996,25 +3990,25 @@
         <v>130</v>
       </c>
       <c r="B124" s="0" t="n">
-        <v>2997.937</v>
+        <v>3068.314</v>
       </c>
       <c r="C124" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D124" s="0" t="n">
-        <v>43.736</v>
+        <v>44.069</v>
       </c>
       <c r="E124" s="0" t="n">
-        <v>2.256</v>
+        <v>2.416</v>
       </c>
       <c r="F124" s="0" t="n">
-        <v>4.549</v>
+        <v>5.918</v>
       </c>
       <c r="G124" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H124" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4022,25 +4016,25 @@
         <v>131</v>
       </c>
       <c r="B125" s="0" t="n">
-        <v>2997.937</v>
+        <v>3068.314</v>
       </c>
       <c r="C125" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D125" s="0" t="n">
-        <v>43.736</v>
+        <v>44.069</v>
       </c>
       <c r="E125" s="0" t="n">
-        <v>2.256</v>
+        <v>2.416</v>
       </c>
       <c r="F125" s="0" t="n">
-        <v>4.949</v>
+        <v>5.918</v>
       </c>
       <c r="G125" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H125" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4048,25 +4042,25 @@
         <v>132</v>
       </c>
       <c r="B126" s="0" t="n">
-        <v>2997.937</v>
+        <v>3068.314</v>
       </c>
       <c r="C126" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D126" s="0" t="n">
-        <v>43.736</v>
+        <v>44.292</v>
       </c>
       <c r="E126" s="0" t="n">
-        <v>2.256</v>
+        <v>2.416</v>
       </c>
       <c r="F126" s="0" t="n">
-        <v>4.949</v>
+        <v>5.918</v>
       </c>
       <c r="G126" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H126" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4074,25 +4068,25 @@
         <v>133</v>
       </c>
       <c r="B127" s="0" t="n">
-        <v>2997.937</v>
+        <v>3075.872</v>
       </c>
       <c r="C127" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D127" s="0" t="n">
-        <v>43.736</v>
+        <v>44.292</v>
       </c>
       <c r="E127" s="0" t="n">
-        <v>2.256</v>
+        <v>2.416</v>
       </c>
       <c r="F127" s="0" t="n">
-        <v>4.949</v>
+        <v>5.918</v>
       </c>
       <c r="G127" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H127" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4100,25 +4094,25 @@
         <v>134</v>
       </c>
       <c r="B128" s="0" t="n">
-        <v>2997.937</v>
+        <v>3094.404</v>
       </c>
       <c r="C128" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D128" s="0" t="n">
-        <v>43.736</v>
+        <v>44.292</v>
       </c>
       <c r="E128" s="0" t="n">
-        <v>2.256</v>
+        <v>2.416</v>
       </c>
       <c r="F128" s="0" t="n">
-        <v>4.949</v>
+        <v>5.918</v>
       </c>
       <c r="G128" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H128" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4126,25 +4120,25 @@
         <v>135</v>
       </c>
       <c r="B129" s="0" t="n">
-        <v>3005.43</v>
+        <v>3094.404</v>
       </c>
       <c r="C129" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D129" s="0" t="n">
-        <v>43.736</v>
+        <v>44.292</v>
       </c>
       <c r="E129" s="0" t="n">
-        <v>2.256</v>
+        <v>2.416</v>
       </c>
       <c r="F129" s="0" t="n">
-        <v>4.949</v>
+        <v>5.918</v>
       </c>
       <c r="G129" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H129" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4152,25 +4146,25 @@
         <v>136</v>
       </c>
       <c r="B130" s="0" t="n">
-        <v>3010.782</v>
+        <v>3094.404</v>
       </c>
       <c r="C130" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D130" s="0" t="n">
-        <v>43.736</v>
+        <v>44.292</v>
       </c>
       <c r="E130" s="0" t="n">
-        <v>2.256</v>
+        <v>2.416</v>
       </c>
       <c r="F130" s="0" t="n">
-        <v>4.949</v>
+        <v>5.918</v>
       </c>
       <c r="G130" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H130" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4178,25 +4172,25 @@
         <v>137</v>
       </c>
       <c r="B131" s="0" t="n">
-        <v>3010.782</v>
+        <v>3094.404</v>
       </c>
       <c r="C131" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D131" s="0" t="n">
-        <v>43.736</v>
+        <v>44.292</v>
       </c>
       <c r="E131" s="0" t="n">
-        <v>2.256</v>
+        <v>2.416</v>
       </c>
       <c r="F131" s="0" t="n">
-        <v>4.949</v>
+        <v>5.918</v>
       </c>
       <c r="G131" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H131" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4204,25 +4198,25 @@
         <v>138</v>
       </c>
       <c r="B132" s="0" t="n">
-        <v>3010.782</v>
+        <v>3104.759</v>
       </c>
       <c r="C132" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D132" s="0" t="n">
-        <v>43.971</v>
+        <v>44.292</v>
       </c>
       <c r="E132" s="0" t="n">
-        <v>2.256</v>
+        <v>2.416</v>
       </c>
       <c r="F132" s="0" t="n">
-        <v>4.949</v>
+        <v>5.918</v>
       </c>
       <c r="G132" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H132" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4230,25 +4224,25 @@
         <v>139</v>
       </c>
       <c r="B133" s="0" t="n">
-        <v>3010.782</v>
+        <v>3104.759</v>
       </c>
       <c r="C133" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D133" s="0" t="n">
-        <v>43.971</v>
+        <v>44.292</v>
       </c>
       <c r="E133" s="0" t="n">
-        <v>2.256</v>
+        <v>2.416</v>
       </c>
       <c r="F133" s="0" t="n">
-        <v>5.216</v>
+        <v>5.918</v>
       </c>
       <c r="G133" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H133" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4256,25 +4250,25 @@
         <v>140</v>
       </c>
       <c r="B134" s="0" t="n">
-        <v>3010.782</v>
+        <v>3104.759</v>
       </c>
       <c r="C134" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D134" s="0" t="n">
-        <v>43.971</v>
+        <v>44.292</v>
       </c>
       <c r="E134" s="0" t="n">
-        <v>2.256</v>
+        <v>2.416</v>
       </c>
       <c r="F134" s="0" t="n">
-        <v>5.442</v>
+        <v>5.918</v>
       </c>
       <c r="G134" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H134" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4282,25 +4276,25 @@
         <v>141</v>
       </c>
       <c r="B135" s="0" t="n">
-        <v>3010.782</v>
+        <v>3104.759</v>
       </c>
       <c r="C135" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D135" s="0" t="n">
-        <v>43.971</v>
+        <v>44.292</v>
       </c>
       <c r="E135" s="0" t="n">
-        <v>2.362</v>
+        <v>2.416</v>
       </c>
       <c r="F135" s="0" t="n">
-        <v>5.442</v>
+        <v>5.918</v>
       </c>
       <c r="G135" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H135" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4308,25 +4302,25 @@
         <v>142</v>
       </c>
       <c r="B136" s="0" t="n">
-        <v>3018.213</v>
+        <v>3104.759</v>
       </c>
       <c r="C136" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D136" s="0" t="n">
-        <v>43.971</v>
+        <v>44.292</v>
       </c>
       <c r="E136" s="0" t="n">
-        <v>2.362</v>
+        <v>2.416</v>
       </c>
       <c r="F136" s="0" t="n">
-        <v>5.442</v>
+        <v>5.918</v>
       </c>
       <c r="G136" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H136" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4334,25 +4328,25 @@
         <v>143</v>
       </c>
       <c r="B137" s="0" t="n">
-        <v>3027.483</v>
+        <v>3104.759</v>
       </c>
       <c r="C137" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D137" s="0" t="n">
-        <v>43.971</v>
+        <v>44.292</v>
       </c>
       <c r="E137" s="0" t="n">
-        <v>2.362</v>
+        <v>2.416</v>
       </c>
       <c r="F137" s="0" t="n">
-        <v>5.442</v>
+        <v>5.918</v>
       </c>
       <c r="G137" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H137" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4360,25 +4354,25 @@
         <v>144</v>
       </c>
       <c r="B138" s="0" t="n">
-        <v>3037.77</v>
+        <v>3104.759</v>
       </c>
       <c r="C138" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D138" s="0" t="n">
-        <v>43.971</v>
+        <v>44.292</v>
       </c>
       <c r="E138" s="0" t="n">
-        <v>2.362</v>
+        <v>2.416</v>
       </c>
       <c r="F138" s="0" t="n">
-        <v>5.442</v>
+        <v>5.918</v>
       </c>
       <c r="G138" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H138" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4386,25 +4380,25 @@
         <v>145</v>
       </c>
       <c r="B139" s="0" t="n">
-        <v>3037.77</v>
+        <v>3104.759</v>
       </c>
       <c r="C139" s="0" t="n">
         <v>164.049</v>
       </c>
       <c r="D139" s="0" t="n">
-        <v>43.971</v>
+        <v>44.292</v>
       </c>
       <c r="E139" s="0" t="n">
-        <v>2.362</v>
+        <v>2.416</v>
       </c>
       <c r="F139" s="0" t="n">
-        <v>5.442</v>
+        <v>5.918</v>
       </c>
       <c r="G139" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H139" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4412,25 +4406,25 @@
         <v>146</v>
       </c>
       <c r="B140" s="0" t="n">
-        <v>3037.77</v>
+        <v>3104.786</v>
       </c>
       <c r="C140" s="0" t="n">
-        <v>164.049</v>
+        <v>164.093</v>
       </c>
       <c r="D140" s="0" t="n">
-        <v>43.971</v>
+        <v>44.292</v>
       </c>
       <c r="E140" s="0" t="n">
-        <v>2.362</v>
+        <v>2.416</v>
       </c>
       <c r="F140" s="0" t="n">
-        <v>5.442</v>
+        <v>5.918</v>
       </c>
       <c r="G140" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H140" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4438,25 +4432,25 @@
         <v>147</v>
       </c>
       <c r="B141" s="0" t="n">
-        <v>3037.77</v>
+        <v>3104.798</v>
       </c>
       <c r="C141" s="0" t="n">
-        <v>164.049</v>
+        <v>164.093</v>
       </c>
       <c r="D141" s="0" t="n">
-        <v>43.979</v>
+        <v>44.292</v>
       </c>
       <c r="E141" s="0" t="n">
-        <v>2.362</v>
+        <v>2.416</v>
       </c>
       <c r="F141" s="0" t="n">
-        <v>5.442</v>
+        <v>5.918</v>
       </c>
       <c r="G141" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H141" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4464,25 +4458,25 @@
         <v>148</v>
       </c>
       <c r="B142" s="0" t="n">
-        <v>3045.333</v>
+        <v>3104.798</v>
       </c>
       <c r="C142" s="0" t="n">
-        <v>164.049</v>
+        <v>164.093</v>
       </c>
       <c r="D142" s="0" t="n">
-        <v>43.979</v>
+        <v>44.292</v>
       </c>
       <c r="E142" s="0" t="n">
-        <v>2.362</v>
+        <v>2.416</v>
       </c>
       <c r="F142" s="0" t="n">
-        <v>5.442</v>
+        <v>5.918</v>
       </c>
       <c r="G142" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H142" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4490,25 +4484,25 @@
         <v>149</v>
       </c>
       <c r="B143" s="0" t="n">
-        <v>3067.38</v>
+        <v>3104.798</v>
       </c>
       <c r="C143" s="0" t="n">
-        <v>164.049</v>
+        <v>164.093</v>
       </c>
       <c r="D143" s="0" t="n">
-        <v>43.979</v>
+        <v>44.292</v>
       </c>
       <c r="E143" s="0" t="n">
-        <v>2.362</v>
+        <v>2.416</v>
       </c>
       <c r="F143" s="0" t="n">
-        <v>5.442</v>
+        <v>5.918</v>
       </c>
       <c r="G143" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H143" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4516,25 +4510,25 @@
         <v>150</v>
       </c>
       <c r="B144" s="0" t="n">
-        <v>3067.38</v>
+        <v>3104.798</v>
       </c>
       <c r="C144" s="0" t="n">
-        <v>164.049</v>
+        <v>164.093</v>
       </c>
       <c r="D144" s="0" t="n">
-        <v>44.017</v>
+        <v>44.292</v>
       </c>
       <c r="E144" s="0" t="n">
         <v>2.416</v>
       </c>
       <c r="F144" s="0" t="n">
-        <v>5.442</v>
+        <v>5.918</v>
       </c>
       <c r="G144" s="0" t="n">
         <v>1.188</v>
       </c>
       <c r="H144" s="0" t="n">
-        <v>1873.577</v>
+        <v>1924.316</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4542,19 +4536,19 @@
         <v>151</v>
       </c>
       <c r="B145" s="0" t="n">
-        <v>3067.38</v>
+        <v>3104.798</v>
       </c>
       <c r="C145" s="0" t="n">
-        <v>164.049</v>
+        <v>164.093</v>
       </c>
       <c r="D145" s="0" t="n">
-        <v>44.069</v>
+        <v>44.292</v>
       </c>
       <c r="E145" s="0" t="n">
         <v>2.416</v>
       </c>
       <c r="F145" s="0" t="n">
-        <v>5.442</v>
+        <v>5.918</v>
       </c>
       <c r="G145" s="0" t="n">
         <v>1.188</v>
@@ -4568,19 +4562,19 @@
         <v>152</v>
       </c>
       <c r="B146" s="0" t="n">
-        <v>3067.38</v>
+        <v>3104.798</v>
       </c>
       <c r="C146" s="0" t="n">
-        <v>164.049</v>
+        <v>164.093</v>
       </c>
       <c r="D146" s="0" t="n">
-        <v>44.069</v>
+        <v>44.292</v>
       </c>
       <c r="E146" s="0" t="n">
         <v>2.416</v>
       </c>
       <c r="F146" s="0" t="n">
-        <v>5.442</v>
+        <v>5.918</v>
       </c>
       <c r="G146" s="0" t="n">
         <v>1.188</v>
@@ -4594,19 +4588,19 @@
         <v>153</v>
       </c>
       <c r="B147" s="0" t="n">
-        <v>3067.856</v>
+        <v>3104.798</v>
       </c>
       <c r="C147" s="0" t="n">
-        <v>164.049</v>
+        <v>164.093</v>
       </c>
       <c r="D147" s="0" t="n">
-        <v>44.069</v>
+        <v>44.292</v>
       </c>
       <c r="E147" s="0" t="n">
         <v>2.416</v>
       </c>
       <c r="F147" s="0" t="n">
-        <v>5.442</v>
+        <v>5.918</v>
       </c>
       <c r="G147" s="0" t="n">
         <v>1.188</v>
@@ -4620,19 +4614,19 @@
         <v>154</v>
       </c>
       <c r="B148" s="0" t="n">
-        <v>3068.084</v>
+        <v>3104.798</v>
       </c>
       <c r="C148" s="0" t="n">
-        <v>164.049</v>
+        <v>164.093</v>
       </c>
       <c r="D148" s="0" t="n">
-        <v>44.069</v>
+        <v>44.292</v>
       </c>
       <c r="E148" s="0" t="n">
         <v>2.416</v>
       </c>
       <c r="F148" s="0" t="n">
-        <v>5.442</v>
+        <v>5.918</v>
       </c>
       <c r="G148" s="0" t="n">
         <v>1.188</v>
@@ -4646,19 +4640,19 @@
         <v>155</v>
       </c>
       <c r="B149" s="0" t="n">
-        <v>3068.314</v>
+        <v>3104.798</v>
       </c>
       <c r="C149" s="0" t="n">
-        <v>164.049</v>
+        <v>164.093</v>
       </c>
       <c r="D149" s="0" t="n">
-        <v>44.069</v>
+        <v>44.292</v>
       </c>
       <c r="E149" s="0" t="n">
         <v>2.416</v>
       </c>
       <c r="F149" s="0" t="n">
-        <v>5.442</v>
+        <v>5.918</v>
       </c>
       <c r="G149" s="0" t="n">
         <v>1.188</v>
@@ -4672,19 +4666,19 @@
         <v>156</v>
       </c>
       <c r="B150" s="0" t="n">
-        <v>3068.314</v>
+        <v>3104.798</v>
       </c>
       <c r="C150" s="0" t="n">
-        <v>164.049</v>
+        <v>164.093</v>
       </c>
       <c r="D150" s="0" t="n">
-        <v>44.069</v>
+        <v>44.292</v>
       </c>
       <c r="E150" s="0" t="n">
         <v>2.416</v>
       </c>
       <c r="F150" s="0" t="n">
-        <v>5.442</v>
+        <v>5.918</v>
       </c>
       <c r="G150" s="0" t="n">
         <v>1.188</v>
@@ -4698,19 +4692,19 @@
         <v>157</v>
       </c>
       <c r="B151" s="0" t="n">
-        <v>3068.314</v>
+        <v>3104.798</v>
       </c>
       <c r="C151" s="0" t="n">
-        <v>164.049</v>
+        <v>164.093</v>
       </c>
       <c r="D151" s="0" t="n">
-        <v>44.069</v>
+        <v>44.292</v>
       </c>
       <c r="E151" s="0" t="n">
         <v>2.416</v>
       </c>
       <c r="F151" s="0" t="n">
-        <v>5.69</v>
+        <v>5.918</v>
       </c>
       <c r="G151" s="0" t="n">
         <v>1.188</v>
@@ -4724,13 +4718,13 @@
         <v>158</v>
       </c>
       <c r="B152" s="0" t="n">
-        <v>3068.314</v>
+        <v>3104.798</v>
       </c>
       <c r="C152" s="0" t="n">
-        <v>164.049</v>
+        <v>164.093</v>
       </c>
       <c r="D152" s="0" t="n">
-        <v>44.069</v>
+        <v>44.292</v>
       </c>
       <c r="E152" s="0" t="n">
         <v>2.416</v>
@@ -4750,13 +4744,13 @@
         <v>159</v>
       </c>
       <c r="B153" s="0" t="n">
-        <v>3068.314</v>
+        <v>3104.798</v>
       </c>
       <c r="C153" s="0" t="n">
-        <v>164.049</v>
+        <v>164.093</v>
       </c>
       <c r="D153" s="0" t="n">
-        <v>44.069</v>
+        <v>44.292</v>
       </c>
       <c r="E153" s="0" t="n">
         <v>2.416</v>
@@ -4776,10 +4770,10 @@
         <v>160</v>
       </c>
       <c r="B154" s="0" t="n">
-        <v>3068.314</v>
+        <v>3104.798</v>
       </c>
       <c r="C154" s="0" t="n">
-        <v>164.049</v>
+        <v>164.093</v>
       </c>
       <c r="D154" s="0" t="n">
         <v>44.292</v>
@@ -4802,10 +4796,10 @@
         <v>161</v>
       </c>
       <c r="B155" s="0" t="n">
-        <v>3075.872</v>
+        <v>3104.798</v>
       </c>
       <c r="C155" s="0" t="n">
-        <v>164.049</v>
+        <v>164.203</v>
       </c>
       <c r="D155" s="0" t="n">
         <v>44.292</v>
@@ -4828,10 +4822,10 @@
         <v>162</v>
       </c>
       <c r="B156" s="0" t="n">
-        <v>3094.404</v>
+        <v>3104.798</v>
       </c>
       <c r="C156" s="0" t="n">
-        <v>164.049</v>
+        <v>164.203</v>
       </c>
       <c r="D156" s="0" t="n">
         <v>44.292</v>
@@ -4854,10 +4848,10 @@
         <v>163</v>
       </c>
       <c r="B157" s="0" t="n">
-        <v>3094.404</v>
+        <v>3104.798</v>
       </c>
       <c r="C157" s="0" t="n">
-        <v>164.049</v>
+        <v>164.203</v>
       </c>
       <c r="D157" s="0" t="n">
         <v>44.292</v>
@@ -4880,10 +4874,10 @@
         <v>164</v>
       </c>
       <c r="B158" s="0" t="n">
-        <v>3094.404</v>
+        <v>3104.798</v>
       </c>
       <c r="C158" s="0" t="n">
-        <v>164.049</v>
+        <v>164.203</v>
       </c>
       <c r="D158" s="0" t="n">
         <v>44.292</v>
@@ -4906,10 +4900,10 @@
         <v>165</v>
       </c>
       <c r="B159" s="0" t="n">
-        <v>3094.404</v>
+        <v>3104.798</v>
       </c>
       <c r="C159" s="0" t="n">
-        <v>164.049</v>
+        <v>164.203</v>
       </c>
       <c r="D159" s="0" t="n">
         <v>44.292</v>
@@ -4932,10 +4926,10 @@
         <v>166</v>
       </c>
       <c r="B160" s="0" t="n">
-        <v>3104.759</v>
+        <v>3104.798</v>
       </c>
       <c r="C160" s="0" t="n">
-        <v>164.049</v>
+        <v>164.203</v>
       </c>
       <c r="D160" s="0" t="n">
         <v>44.292</v>
@@ -4958,10 +4952,10 @@
         <v>167</v>
       </c>
       <c r="B161" s="0" t="n">
-        <v>3104.759</v>
+        <v>3104.808</v>
       </c>
       <c r="C161" s="0" t="n">
-        <v>164.049</v>
+        <v>164.247</v>
       </c>
       <c r="D161" s="0" t="n">
         <v>44.292</v>
@@ -4984,10 +4978,10 @@
         <v>168</v>
       </c>
       <c r="B162" s="0" t="n">
-        <v>3104.759</v>
+        <v>3104.808</v>
       </c>
       <c r="C162" s="0" t="n">
-        <v>164.049</v>
+        <v>164.247</v>
       </c>
       <c r="D162" s="0" t="n">
         <v>44.292</v>
@@ -5010,10 +5004,10 @@
         <v>169</v>
       </c>
       <c r="B163" s="0" t="n">
-        <v>3104.759</v>
+        <v>3104.808</v>
       </c>
       <c r="C163" s="0" t="n">
-        <v>164.049</v>
+        <v>164.247</v>
       </c>
       <c r="D163" s="0" t="n">
         <v>44.292</v>
@@ -5036,10 +5030,10 @@
         <v>170</v>
       </c>
       <c r="B164" s="0" t="n">
-        <v>3104.759</v>
+        <v>3104.808</v>
       </c>
       <c r="C164" s="0" t="n">
-        <v>164.049</v>
+        <v>164.247</v>
       </c>
       <c r="D164" s="0" t="n">
         <v>44.292</v>
@@ -5062,10 +5056,10 @@
         <v>171</v>
       </c>
       <c r="B165" s="0" t="n">
-        <v>3104.759</v>
+        <v>3104.808</v>
       </c>
       <c r="C165" s="0" t="n">
-        <v>164.049</v>
+        <v>164.247</v>
       </c>
       <c r="D165" s="0" t="n">
         <v>44.292</v>
@@ -5088,10 +5082,10 @@
         <v>172</v>
       </c>
       <c r="B166" s="0" t="n">
-        <v>3104.759</v>
+        <v>3104.808</v>
       </c>
       <c r="C166" s="0" t="n">
-        <v>164.049</v>
+        <v>164.247</v>
       </c>
       <c r="D166" s="0" t="n">
         <v>44.292</v>
@@ -5114,10 +5108,10 @@
         <v>173</v>
       </c>
       <c r="B167" s="0" t="n">
-        <v>3104.759</v>
+        <v>3104.808</v>
       </c>
       <c r="C167" s="0" t="n">
-        <v>164.049</v>
+        <v>164.247</v>
       </c>
       <c r="D167" s="0" t="n">
         <v>44.292</v>
@@ -5140,10 +5134,10 @@
         <v>174</v>
       </c>
       <c r="B168" s="0" t="n">
-        <v>3104.786</v>
+        <v>3104.808</v>
       </c>
       <c r="C168" s="0" t="n">
-        <v>164.093</v>
+        <v>164.247</v>
       </c>
       <c r="D168" s="0" t="n">
         <v>44.292</v>
@@ -5166,10 +5160,10 @@
         <v>175</v>
       </c>
       <c r="B169" s="0" t="n">
-        <v>3104.798</v>
+        <v>3104.808</v>
       </c>
       <c r="C169" s="0" t="n">
-        <v>164.093</v>
+        <v>164.249</v>
       </c>
       <c r="D169" s="0" t="n">
         <v>44.292</v>
@@ -5192,10 +5186,10 @@
         <v>176</v>
       </c>
       <c r="B170" s="0" t="n">
-        <v>3104.798</v>
+        <v>3104.808</v>
       </c>
       <c r="C170" s="0" t="n">
-        <v>164.093</v>
+        <v>164.249</v>
       </c>
       <c r="D170" s="0" t="n">
         <v>44.292</v>
@@ -5218,10 +5212,10 @@
         <v>177</v>
       </c>
       <c r="B171" s="0" t="n">
-        <v>3104.798</v>
+        <v>3104.808</v>
       </c>
       <c r="C171" s="0" t="n">
-        <v>164.093</v>
+        <v>164.249</v>
       </c>
       <c r="D171" s="0" t="n">
         <v>44.292</v>
@@ -5244,10 +5238,10 @@
         <v>178</v>
       </c>
       <c r="B172" s="0" t="n">
-        <v>3104.798</v>
+        <v>3104.808</v>
       </c>
       <c r="C172" s="0" t="n">
-        <v>164.093</v>
+        <v>164.249</v>
       </c>
       <c r="D172" s="0" t="n">
         <v>44.292</v>
@@ -5270,10 +5264,10 @@
         <v>179</v>
       </c>
       <c r="B173" s="0" t="n">
-        <v>3104.798</v>
+        <v>3104.808</v>
       </c>
       <c r="C173" s="0" t="n">
-        <v>164.093</v>
+        <v>164.249</v>
       </c>
       <c r="D173" s="0" t="n">
         <v>44.292</v>
@@ -5296,10 +5290,10 @@
         <v>180</v>
       </c>
       <c r="B174" s="0" t="n">
-        <v>3104.798</v>
+        <v>3104.808</v>
       </c>
       <c r="C174" s="0" t="n">
-        <v>164.093</v>
+        <v>164.249</v>
       </c>
       <c r="D174" s="0" t="n">
         <v>44.292</v>
@@ -5322,10 +5316,10 @@
         <v>181</v>
       </c>
       <c r="B175" s="0" t="n">
-        <v>3104.798</v>
+        <v>3104.808</v>
       </c>
       <c r="C175" s="0" t="n">
-        <v>164.093</v>
+        <v>164.249</v>
       </c>
       <c r="D175" s="0" t="n">
         <v>44.292</v>
@@ -5348,10 +5342,10 @@
         <v>182</v>
       </c>
       <c r="B176" s="0" t="n">
-        <v>3104.798</v>
+        <v>3104.808</v>
       </c>
       <c r="C176" s="0" t="n">
-        <v>164.093</v>
+        <v>164.249</v>
       </c>
       <c r="D176" s="0" t="n">
         <v>44.292</v>
@@ -5374,10 +5368,10 @@
         <v>183</v>
       </c>
       <c r="B177" s="0" t="n">
-        <v>3104.798</v>
+        <v>3104.808</v>
       </c>
       <c r="C177" s="0" t="n">
-        <v>164.093</v>
+        <v>164.249</v>
       </c>
       <c r="D177" s="0" t="n">
         <v>44.292</v>
@@ -5400,10 +5394,10 @@
         <v>184</v>
       </c>
       <c r="B178" s="0" t="n">
-        <v>3104.798</v>
+        <v>3104.808</v>
       </c>
       <c r="C178" s="0" t="n">
-        <v>164.093</v>
+        <v>164.249</v>
       </c>
       <c r="D178" s="0" t="n">
         <v>44.292</v>
@@ -5426,10 +5420,10 @@
         <v>185</v>
       </c>
       <c r="B179" s="0" t="n">
-        <v>3104.798</v>
+        <v>3104.808</v>
       </c>
       <c r="C179" s="0" t="n">
-        <v>164.093</v>
+        <v>164.249</v>
       </c>
       <c r="D179" s="0" t="n">
         <v>44.292</v>
@@ -5452,10 +5446,10 @@
         <v>186</v>
       </c>
       <c r="B180" s="0" t="n">
-        <v>3104.798</v>
+        <v>3104.808</v>
       </c>
       <c r="C180" s="0" t="n">
-        <v>164.093</v>
+        <v>164.249</v>
       </c>
       <c r="D180" s="0" t="n">
         <v>44.292</v>
@@ -5478,10 +5472,10 @@
         <v>187</v>
       </c>
       <c r="B181" s="0" t="n">
-        <v>3104.798</v>
+        <v>3104.808</v>
       </c>
       <c r="C181" s="0" t="n">
-        <v>164.093</v>
+        <v>164.249</v>
       </c>
       <c r="D181" s="0" t="n">
         <v>44.292</v>
@@ -5504,10 +5498,10 @@
         <v>188</v>
       </c>
       <c r="B182" s="0" t="n">
-        <v>3104.798</v>
+        <v>3104.808</v>
       </c>
       <c r="C182" s="0" t="n">
-        <v>164.093</v>
+        <v>164.249</v>
       </c>
       <c r="D182" s="0" t="n">
         <v>44.292</v>
@@ -5530,10 +5524,10 @@
         <v>189</v>
       </c>
       <c r="B183" s="0" t="n">
-        <v>3104.798</v>
+        <v>3104.808</v>
       </c>
       <c r="C183" s="0" t="n">
-        <v>164.203</v>
+        <v>164.249</v>
       </c>
       <c r="D183" s="0" t="n">
         <v>44.292</v>
@@ -5556,10 +5550,10 @@
         <v>190</v>
       </c>
       <c r="B184" s="0" t="n">
-        <v>3104.798</v>
+        <v>3119.148</v>
       </c>
       <c r="C184" s="0" t="n">
-        <v>164.203</v>
+        <v>182.007</v>
       </c>
       <c r="D184" s="0" t="n">
         <v>44.292</v>
@@ -5582,10 +5576,10 @@
         <v>191</v>
       </c>
       <c r="B185" s="0" t="n">
-        <v>3104.798</v>
+        <v>3124.194</v>
       </c>
       <c r="C185" s="0" t="n">
-        <v>164.203</v>
+        <v>182.007</v>
       </c>
       <c r="D185" s="0" t="n">
         <v>44.292</v>
@@ -5608,10 +5602,10 @@
         <v>192</v>
       </c>
       <c r="B186" s="0" t="n">
-        <v>3104.798</v>
+        <v>3124.194</v>
       </c>
       <c r="C186" s="0" t="n">
-        <v>164.203</v>
+        <v>182.007</v>
       </c>
       <c r="D186" s="0" t="n">
         <v>44.292</v>
@@ -5634,10 +5628,10 @@
         <v>193</v>
       </c>
       <c r="B187" s="0" t="n">
-        <v>3104.798</v>
+        <v>3124.194</v>
       </c>
       <c r="C187" s="0" t="n">
-        <v>164.203</v>
+        <v>182.007</v>
       </c>
       <c r="D187" s="0" t="n">
         <v>44.292</v>
@@ -5660,10 +5654,10 @@
         <v>194</v>
       </c>
       <c r="B188" s="0" t="n">
-        <v>3104.798</v>
+        <v>3124.194</v>
       </c>
       <c r="C188" s="0" t="n">
-        <v>164.203</v>
+        <v>182.007</v>
       </c>
       <c r="D188" s="0" t="n">
         <v>44.292</v>
@@ -5686,10 +5680,10 @@
         <v>195</v>
       </c>
       <c r="B189" s="0" t="n">
-        <v>3104.808</v>
+        <v>3124.682</v>
       </c>
       <c r="C189" s="0" t="n">
-        <v>164.247</v>
+        <v>182.007</v>
       </c>
       <c r="D189" s="0" t="n">
         <v>44.292</v>
@@ -5712,10 +5706,10 @@
         <v>196</v>
       </c>
       <c r="B190" s="0" t="n">
-        <v>3104.808</v>
+        <v>3140.801</v>
       </c>
       <c r="C190" s="0" t="n">
-        <v>164.247</v>
+        <v>187.483</v>
       </c>
       <c r="D190" s="0" t="n">
         <v>44.292</v>
@@ -5738,10 +5732,10 @@
         <v>197</v>
       </c>
       <c r="B191" s="0" t="n">
-        <v>3104.808</v>
+        <v>3140.801</v>
       </c>
       <c r="C191" s="0" t="n">
-        <v>164.247</v>
+        <v>187.483</v>
       </c>
       <c r="D191" s="0" t="n">
         <v>44.292</v>
@@ -5764,10 +5758,10 @@
         <v>198</v>
       </c>
       <c r="B192" s="0" t="n">
-        <v>3104.808</v>
+        <v>3140.801</v>
       </c>
       <c r="C192" s="0" t="n">
-        <v>164.247</v>
+        <v>187.483</v>
       </c>
       <c r="D192" s="0" t="n">
         <v>44.292</v>
@@ -5790,10 +5784,10 @@
         <v>199</v>
       </c>
       <c r="B193" s="0" t="n">
-        <v>3104.808</v>
+        <v>3140.801</v>
       </c>
       <c r="C193" s="0" t="n">
-        <v>164.247</v>
+        <v>187.483</v>
       </c>
       <c r="D193" s="0" t="n">
         <v>44.292</v>
@@ -5816,10 +5810,10 @@
         <v>200</v>
       </c>
       <c r="B194" s="0" t="n">
-        <v>3104.808</v>
+        <v>3140.961</v>
       </c>
       <c r="C194" s="0" t="n">
-        <v>164.247</v>
+        <v>187.483</v>
       </c>
       <c r="D194" s="0" t="n">
         <v>44.292</v>
@@ -5842,10 +5836,10 @@
         <v>201</v>
       </c>
       <c r="B195" s="0" t="n">
-        <v>3104.808</v>
+        <v>3140.961</v>
       </c>
       <c r="C195" s="0" t="n">
-        <v>164.247</v>
+        <v>187.483</v>
       </c>
       <c r="D195" s="0" t="n">
         <v>44.292</v>
@@ -5868,10 +5862,10 @@
         <v>202</v>
       </c>
       <c r="B196" s="0" t="n">
-        <v>3104.808</v>
+        <v>3148.376</v>
       </c>
       <c r="C196" s="0" t="n">
-        <v>164.247</v>
+        <v>198.064</v>
       </c>
       <c r="D196" s="0" t="n">
         <v>44.292</v>
@@ -5894,10 +5888,10 @@
         <v>203</v>
       </c>
       <c r="B197" s="0" t="n">
-        <v>3104.808</v>
+        <v>3169.944</v>
       </c>
       <c r="C197" s="0" t="n">
-        <v>164.249</v>
+        <v>198.064</v>
       </c>
       <c r="D197" s="0" t="n">
         <v>44.292</v>
@@ -5920,10 +5914,10 @@
         <v>204</v>
       </c>
       <c r="B198" s="0" t="n">
-        <v>3104.808</v>
+        <v>3192.78</v>
       </c>
       <c r="C198" s="0" t="n">
-        <v>164.249</v>
+        <v>200.548</v>
       </c>
       <c r="D198" s="0" t="n">
         <v>44.292</v>
@@ -5946,10 +5940,10 @@
         <v>205</v>
       </c>
       <c r="B199" s="0" t="n">
-        <v>3104.808</v>
+        <v>3192.78</v>
       </c>
       <c r="C199" s="0" t="n">
-        <v>164.249</v>
+        <v>200.548</v>
       </c>
       <c r="D199" s="0" t="n">
         <v>44.292</v>
@@ -5972,10 +5966,10 @@
         <v>206</v>
       </c>
       <c r="B200" s="0" t="n">
-        <v>3104.808</v>
+        <v>3192.78</v>
       </c>
       <c r="C200" s="0" t="n">
-        <v>164.249</v>
+        <v>200.548</v>
       </c>
       <c r="D200" s="0" t="n">
         <v>44.292</v>
@@ -5998,10 +5992,10 @@
         <v>207</v>
       </c>
       <c r="B201" s="0" t="n">
-        <v>3104.808</v>
+        <v>3192.78</v>
       </c>
       <c r="C201" s="0" t="n">
-        <v>164.249</v>
+        <v>200.548</v>
       </c>
       <c r="D201" s="0" t="n">
         <v>44.292</v>
@@ -6024,10 +6018,10 @@
         <v>208</v>
       </c>
       <c r="B202" s="0" t="n">
-        <v>3104.808</v>
+        <v>3192.78</v>
       </c>
       <c r="C202" s="0" t="n">
-        <v>164.249</v>
+        <v>200.548</v>
       </c>
       <c r="D202" s="0" t="n">
         <v>44.292</v>
@@ -6050,10 +6044,10 @@
         <v>209</v>
       </c>
       <c r="B203" s="0" t="n">
-        <v>3104.808</v>
+        <v>3192.781</v>
       </c>
       <c r="C203" s="0" t="n">
-        <v>164.249</v>
+        <v>200.548</v>
       </c>
       <c r="D203" s="0" t="n">
         <v>44.292</v>
@@ -6076,10 +6070,10 @@
         <v>210</v>
       </c>
       <c r="B204" s="0" t="n">
-        <v>3104.808</v>
+        <v>3193.215</v>
       </c>
       <c r="C204" s="0" t="n">
-        <v>164.249</v>
+        <v>200.548</v>
       </c>
       <c r="D204" s="0" t="n">
         <v>44.292</v>
@@ -6102,10 +6096,10 @@
         <v>211</v>
       </c>
       <c r="B205" s="0" t="n">
-        <v>3104.808</v>
+        <v>3193.215</v>
       </c>
       <c r="C205" s="0" t="n">
-        <v>164.249</v>
+        <v>200.548</v>
       </c>
       <c r="D205" s="0" t="n">
         <v>44.292</v>
@@ -6128,10 +6122,10 @@
         <v>212</v>
       </c>
       <c r="B206" s="0" t="n">
-        <v>3104.808</v>
+        <v>3193.215</v>
       </c>
       <c r="C206" s="0" t="n">
-        <v>164.249</v>
+        <v>200.548</v>
       </c>
       <c r="D206" s="0" t="n">
         <v>44.292</v>
@@ -6154,10 +6148,10 @@
         <v>213</v>
       </c>
       <c r="B207" s="0" t="n">
-        <v>3104.808</v>
+        <v>3193.215</v>
       </c>
       <c r="C207" s="0" t="n">
-        <v>164.249</v>
+        <v>200.548</v>
       </c>
       <c r="D207" s="0" t="n">
         <v>44.292</v>
@@ -6180,10 +6174,10 @@
         <v>214</v>
       </c>
       <c r="B208" s="0" t="n">
-        <v>3104.808</v>
+        <v>3193.215</v>
       </c>
       <c r="C208" s="0" t="n">
-        <v>164.249</v>
+        <v>200.961</v>
       </c>
       <c r="D208" s="0" t="n">
         <v>44.292</v>
@@ -6206,10 +6200,10 @@
         <v>215</v>
       </c>
       <c r="B209" s="0" t="n">
-        <v>3104.808</v>
+        <v>3193.517</v>
       </c>
       <c r="C209" s="0" t="n">
-        <v>164.249</v>
+        <v>200.961</v>
       </c>
       <c r="D209" s="0" t="n">
         <v>44.292</v>
@@ -6232,10 +6226,10 @@
         <v>216</v>
       </c>
       <c r="B210" s="0" t="n">
-        <v>3104.808</v>
+        <v>3193.517</v>
       </c>
       <c r="C210" s="0" t="n">
-        <v>164.249</v>
+        <v>200.961</v>
       </c>
       <c r="D210" s="0" t="n">
         <v>44.292</v>
@@ -6250,58 +6244,6 @@
         <v>1.188</v>
       </c>
       <c r="H210" s="0" t="n">
-        <v>1924.316</v>
-      </c>
-    </row>
-    <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A211" s="0" t="s">
-        <v>217</v>
-      </c>
-      <c r="B211" s="0" t="n">
-        <v>3104.808</v>
-      </c>
-      <c r="C211" s="0" t="n">
-        <v>164.249</v>
-      </c>
-      <c r="D211" s="0" t="n">
-        <v>44.292</v>
-      </c>
-      <c r="E211" s="0" t="n">
-        <v>2.416</v>
-      </c>
-      <c r="F211" s="0" t="n">
-        <v>5.918</v>
-      </c>
-      <c r="G211" s="0" t="n">
-        <v>1.188</v>
-      </c>
-      <c r="H211" s="0" t="n">
-        <v>1924.316</v>
-      </c>
-    </row>
-    <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A212" s="0" t="s">
-        <v>218</v>
-      </c>
-      <c r="B212" s="0" t="n">
-        <v>3119.148</v>
-      </c>
-      <c r="C212" s="0" t="n">
-        <v>182.007</v>
-      </c>
-      <c r="D212" s="0" t="n">
-        <v>44.292</v>
-      </c>
-      <c r="E212" s="0" t="n">
-        <v>2.416</v>
-      </c>
-      <c r="F212" s="0" t="n">
-        <v>5.918</v>
-      </c>
-      <c r="G212" s="0" t="n">
-        <v>1.188</v>
-      </c>
-      <c r="H212" s="0" t="n">
         <v>1924.316</v>
       </c>
     </row>

</xml_diff>